<commit_message>
First working version - need tests
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/registration_datahub/tests/test_file/new_reg_data_import.xlsx
+++ b/backend/hct_mis_api/apps/registration_datahub/tests/test_file/new_reg_data_import.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="238">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -27,10 +27,38 @@
     <t>Excel Worksheet Name</t>
   </si>
   <si>
+    <t>Export Summary</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
     <t>Households</t>
   </si>
   <si>
-    <t>Table 1</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Households</t>
+    </r>
+  </si>
+  <si>
+    <t>Individuals</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Individuals</t>
+    </r>
   </si>
   <si>
     <t>household_id</t>
@@ -384,16 +412,13 @@
     <t>REFUGEE</t>
   </si>
   <si>
-    <t>Afghanistan</t>
+    <t>AF</t>
   </si>
   <si>
     <t>some house 33</t>
   </si>
   <si>
     <t>34.979538, 70.779336</t>
-  </si>
-  <si>
-    <t>Individuals</t>
   </si>
   <si>
     <t>age</t>
@@ -766,7 +791,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -785,13 +810,118 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -815,7 +945,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -837,28 +967,85 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -882,6 +1069,9 @@
       <rgbColor rgb="01eef3f4"/>
       <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ff5e88b1"/>
+      <rgbColor rgb="ffeef3f4"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1220,12 +1410,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1258,10 +1448,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1509,12 +1699,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1829,10 +2019,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2083,73 +2273,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="1" max="1" width="2" style="6" customWidth="1"/>
     <col min="2" max="4" width="30.5547" customWidth="1"/>
+    <col min="2" max="2" width="30.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="30.5" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="10" style="6" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="14.6" customHeight="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" ht="14.6" customHeight="1">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+    </row>
     <row r="3" ht="0.05" customHeight="1">
-      <c r="B3" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="A3" s="10"/>
+      <c r="B3" t="s" s="13">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" ht="14.6" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" ht="14.6" customHeight="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" ht="14.6" customHeight="1">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="A7" s="10"/>
+      <c r="B7" t="s" s="14">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" t="s" s="14">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" t="s" s="14">
         <v>3</v>
       </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" ht="14.6" customHeight="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9">
-      <c r="B9" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="10"/>
+      <c r="B9" t="s" s="15">
+        <v>6</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="A10" s="10"/>
+      <c r="B10" s="17"/>
+      <c r="C10" t="s" s="18">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
-        <v>4</v>
-      </c>
+      <c r="D10" t="s" s="19">
+        <v>7</v>
+      </c>
+      <c r="E10" s="12"/>
     </row>
-    <row r="11">
+    <row r="11" ht="13" customHeight="1">
+      <c r="A11" s="10"/>
       <c r="B11" t="s" s="3">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
+      <c r="E11" s="12"/>
     </row>
-    <row r="12">
+    <row r="12" ht="13" customHeight="1">
+      <c r="A12" s="20"/>
       <c r="B12" s="4"/>
       <c r="C12" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>126</v>
+        <v>6</v>
+      </c>
+      <c r="E12" s="24"/>
+    </row>
+    <row r="13">
+      <c r="B13" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="4"/>
+      <c r="C14" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s" s="5">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
+    <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
     <hyperlink ref="D10" location="'Households'!R1C1" tooltip="" display="Households"/>
     <hyperlink ref="D12" location="'Individuals'!R1C1" tooltip="" display="Individuals"/>
+    <hyperlink ref="D12" location="'Households'!R1C1" tooltip="" display="Households"/>
+    <hyperlink ref="D14" location="'Individuals'!R1C1" tooltip="" display="Individuals"/>
   </hyperlinks>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2161,1050 +2440,1050 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.8516" style="6" customWidth="1"/>
-    <col min="2" max="3" width="20.6719" style="6" customWidth="1"/>
-    <col min="4" max="4" width="15.1719" style="6" customWidth="1"/>
-    <col min="5" max="5" width="10" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12" style="6" customWidth="1"/>
-    <col min="7" max="8" width="37.8516" style="6" customWidth="1"/>
-    <col min="9" max="9" width="17.3516" style="6" customWidth="1"/>
-    <col min="10" max="10" width="13.6719" style="6" customWidth="1"/>
-    <col min="11" max="11" width="22.1719" style="6" customWidth="1"/>
-    <col min="12" max="12" width="21.3516" style="6" customWidth="1"/>
-    <col min="13" max="13" width="49.8516" style="6" customWidth="1"/>
-    <col min="14" max="14" width="20.5" style="6" customWidth="1"/>
-    <col min="15" max="15" width="21.3516" style="6" customWidth="1"/>
-    <col min="16" max="16" width="22.3516" style="6" customWidth="1"/>
-    <col min="17" max="17" width="18.8516" style="6" customWidth="1"/>
-    <col min="18" max="18" width="21.3516" style="6" customWidth="1"/>
-    <col min="19" max="19" width="18.8516" style="6" customWidth="1"/>
-    <col min="20" max="20" width="19.8516" style="6" customWidth="1"/>
-    <col min="21" max="21" width="20.6719" style="6" customWidth="1"/>
-    <col min="22" max="22" width="17.3516" style="6" customWidth="1"/>
-    <col min="23" max="23" width="37.5" style="6" customWidth="1"/>
-    <col min="24" max="24" width="38.3516" style="6" customWidth="1"/>
-    <col min="25" max="25" width="39.3516" style="6" customWidth="1"/>
-    <col min="26" max="26" width="36.6719" style="6" customWidth="1"/>
-    <col min="27" max="27" width="35.8516" style="6" customWidth="1"/>
-    <col min="28" max="28" width="36.8516" style="6" customWidth="1"/>
-    <col min="29" max="29" width="37.8516" style="6" customWidth="1"/>
-    <col min="30" max="30" width="35" style="6" customWidth="1"/>
-    <col min="31" max="31" width="44.8516" style="6" customWidth="1"/>
-    <col min="32" max="32" width="63" style="6" customWidth="1"/>
-    <col min="33" max="33" width="112" style="6" customWidth="1"/>
-    <col min="34" max="34" width="58.8516" style="6" customWidth="1"/>
-    <col min="35" max="35" width="31" style="6" customWidth="1"/>
-    <col min="36" max="36" width="22.1719" style="6" customWidth="1"/>
-    <col min="37" max="37" width="22" style="6" customWidth="1"/>
-    <col min="38" max="38" width="57.3516" style="6" customWidth="1"/>
-    <col min="39" max="39" width="43.5" style="6" customWidth="1"/>
-    <col min="40" max="40" width="71.1719" style="6" customWidth="1"/>
-    <col min="41" max="41" width="39.8516" style="6" customWidth="1"/>
-    <col min="42" max="42" width="35.1719" style="6" customWidth="1"/>
-    <col min="43" max="43" width="39.3516" style="6" customWidth="1"/>
-    <col min="44" max="44" width="17.8516" style="6" customWidth="1"/>
-    <col min="45" max="45" width="41" style="6" customWidth="1"/>
-    <col min="46" max="46" width="48.8516" style="6" customWidth="1"/>
-    <col min="47" max="47" width="41.8516" style="6" customWidth="1"/>
-    <col min="48" max="48" width="33" style="6" customWidth="1"/>
-    <col min="49" max="49" width="43.1719" style="6" customWidth="1"/>
-    <col min="50" max="50" width="25.8516" style="6" customWidth="1"/>
-    <col min="51" max="51" width="62.8516" style="6" customWidth="1"/>
-    <col min="52" max="52" width="34.5" style="6" customWidth="1"/>
-    <col min="53" max="53" width="30.6719" style="6" customWidth="1"/>
-    <col min="54" max="54" width="32.8516" style="6" customWidth="1"/>
-    <col min="55" max="55" width="55.6719" style="6" customWidth="1"/>
-    <col min="56" max="56" width="70.1719" style="6" customWidth="1"/>
-    <col min="57" max="57" width="52.3516" style="6" customWidth="1"/>
-    <col min="58" max="58" width="57.1719" style="6" customWidth="1"/>
-    <col min="59" max="16384" width="12.6719" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.8516" style="25" customWidth="1"/>
+    <col min="2" max="3" width="20.6719" style="25" customWidth="1"/>
+    <col min="4" max="4" width="15.1719" style="25" customWidth="1"/>
+    <col min="5" max="5" width="10" style="25" customWidth="1"/>
+    <col min="6" max="6" width="12" style="25" customWidth="1"/>
+    <col min="7" max="8" width="37.8516" style="25" customWidth="1"/>
+    <col min="9" max="9" width="17.3516" style="25" customWidth="1"/>
+    <col min="10" max="10" width="13.6719" style="25" customWidth="1"/>
+    <col min="11" max="11" width="22.1719" style="25" customWidth="1"/>
+    <col min="12" max="12" width="21.3516" style="25" customWidth="1"/>
+    <col min="13" max="13" width="49.8516" style="25" customWidth="1"/>
+    <col min="14" max="14" width="20.5" style="25" customWidth="1"/>
+    <col min="15" max="15" width="21.3516" style="25" customWidth="1"/>
+    <col min="16" max="16" width="22.3516" style="25" customWidth="1"/>
+    <col min="17" max="17" width="18.8516" style="25" customWidth="1"/>
+    <col min="18" max="18" width="21.3516" style="25" customWidth="1"/>
+    <col min="19" max="19" width="18.8516" style="25" customWidth="1"/>
+    <col min="20" max="20" width="19.8516" style="25" customWidth="1"/>
+    <col min="21" max="21" width="20.6719" style="25" customWidth="1"/>
+    <col min="22" max="22" width="17.3516" style="25" customWidth="1"/>
+    <col min="23" max="23" width="37.5" style="25" customWidth="1"/>
+    <col min="24" max="24" width="38.3516" style="25" customWidth="1"/>
+    <col min="25" max="25" width="39.3516" style="25" customWidth="1"/>
+    <col min="26" max="26" width="36.6719" style="25" customWidth="1"/>
+    <col min="27" max="27" width="35.8516" style="25" customWidth="1"/>
+    <col min="28" max="28" width="36.8516" style="25" customWidth="1"/>
+    <col min="29" max="29" width="37.8516" style="25" customWidth="1"/>
+    <col min="30" max="30" width="35" style="25" customWidth="1"/>
+    <col min="31" max="31" width="44.8516" style="25" customWidth="1"/>
+    <col min="32" max="32" width="63" style="25" customWidth="1"/>
+    <col min="33" max="33" width="112" style="25" customWidth="1"/>
+    <col min="34" max="34" width="58.8516" style="25" customWidth="1"/>
+    <col min="35" max="35" width="31" style="25" customWidth="1"/>
+    <col min="36" max="36" width="22.1719" style="25" customWidth="1"/>
+    <col min="37" max="37" width="22" style="25" customWidth="1"/>
+    <col min="38" max="38" width="57.3516" style="25" customWidth="1"/>
+    <col min="39" max="39" width="43.5" style="25" customWidth="1"/>
+    <col min="40" max="40" width="71.1719" style="25" customWidth="1"/>
+    <col min="41" max="41" width="39.8516" style="25" customWidth="1"/>
+    <col min="42" max="42" width="35.1719" style="25" customWidth="1"/>
+    <col min="43" max="43" width="39.3516" style="25" customWidth="1"/>
+    <col min="44" max="44" width="17.8516" style="25" customWidth="1"/>
+    <col min="45" max="45" width="41" style="25" customWidth="1"/>
+    <col min="46" max="46" width="48.8516" style="25" customWidth="1"/>
+    <col min="47" max="47" width="41.8516" style="25" customWidth="1"/>
+    <col min="48" max="48" width="33" style="25" customWidth="1"/>
+    <col min="49" max="49" width="43.1719" style="25" customWidth="1"/>
+    <col min="50" max="50" width="25.8516" style="25" customWidth="1"/>
+    <col min="51" max="51" width="62.8516" style="25" customWidth="1"/>
+    <col min="52" max="52" width="34.5" style="25" customWidth="1"/>
+    <col min="53" max="53" width="30.6719" style="25" customWidth="1"/>
+    <col min="54" max="54" width="32.8516" style="25" customWidth="1"/>
+    <col min="55" max="55" width="55.6719" style="25" customWidth="1"/>
+    <col min="56" max="56" width="70.1719" style="25" customWidth="1"/>
+    <col min="57" max="57" width="52.3516" style="25" customWidth="1"/>
+    <col min="58" max="58" width="57.1719" style="25" customWidth="1"/>
+    <col min="59" max="16384" width="12.6719" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s" s="7">
+      <c r="A1" t="s" s="26">
         <v>10</v>
       </c>
-      <c r="F1" t="s" s="7">
+      <c r="B1" t="s" s="26">
         <v>11</v>
       </c>
-      <c r="G1" t="s" s="7">
+      <c r="C1" t="s" s="26">
         <v>12</v>
       </c>
-      <c r="H1" t="s" s="7">
+      <c r="D1" t="s" s="26">
         <v>13</v>
       </c>
-      <c r="I1" t="s" s="7">
+      <c r="E1" t="s" s="26">
         <v>14</v>
       </c>
-      <c r="J1" t="s" s="7">
+      <c r="F1" t="s" s="26">
         <v>15</v>
       </c>
-      <c r="K1" t="s" s="7">
+      <c r="G1" t="s" s="26">
         <v>16</v>
       </c>
-      <c r="L1" t="s" s="7">
+      <c r="H1" t="s" s="26">
         <v>17</v>
       </c>
-      <c r="M1" t="s" s="7">
+      <c r="I1" t="s" s="26">
         <v>18</v>
       </c>
-      <c r="N1" t="s" s="7">
+      <c r="J1" t="s" s="26">
         <v>19</v>
       </c>
-      <c r="O1" t="s" s="7">
+      <c r="K1" t="s" s="26">
         <v>20</v>
       </c>
-      <c r="P1" t="s" s="7">
+      <c r="L1" t="s" s="26">
         <v>21</v>
       </c>
-      <c r="Q1" t="s" s="7">
+      <c r="M1" t="s" s="26">
         <v>22</v>
       </c>
-      <c r="R1" t="s" s="7">
+      <c r="N1" t="s" s="26">
         <v>23</v>
       </c>
-      <c r="S1" t="s" s="7">
+      <c r="O1" t="s" s="26">
         <v>24</v>
       </c>
-      <c r="T1" t="s" s="7">
+      <c r="P1" t="s" s="26">
         <v>25</v>
       </c>
-      <c r="U1" t="s" s="7">
+      <c r="Q1" t="s" s="26">
         <v>26</v>
       </c>
-      <c r="V1" t="s" s="7">
+      <c r="R1" t="s" s="26">
         <v>27</v>
       </c>
-      <c r="W1" t="s" s="7">
+      <c r="S1" t="s" s="26">
         <v>28</v>
       </c>
-      <c r="X1" t="s" s="7">
+      <c r="T1" t="s" s="26">
         <v>29</v>
       </c>
-      <c r="Y1" t="s" s="7">
+      <c r="U1" t="s" s="26">
         <v>30</v>
       </c>
-      <c r="Z1" t="s" s="7">
+      <c r="V1" t="s" s="26">
         <v>31</v>
       </c>
-      <c r="AA1" t="s" s="7">
+      <c r="W1" t="s" s="26">
         <v>32</v>
       </c>
-      <c r="AB1" t="s" s="7">
+      <c r="X1" t="s" s="26">
         <v>33</v>
       </c>
-      <c r="AC1" t="s" s="7">
+      <c r="Y1" t="s" s="26">
         <v>34</v>
       </c>
-      <c r="AD1" t="s" s="7">
+      <c r="Z1" t="s" s="26">
         <v>35</v>
       </c>
-      <c r="AE1" t="s" s="7">
+      <c r="AA1" t="s" s="26">
         <v>36</v>
       </c>
-      <c r="AF1" t="s" s="7">
+      <c r="AB1" t="s" s="26">
         <v>37</v>
       </c>
-      <c r="AG1" t="s" s="7">
+      <c r="AC1" t="s" s="26">
         <v>38</v>
       </c>
-      <c r="AH1" t="s" s="7">
+      <c r="AD1" t="s" s="26">
         <v>39</v>
       </c>
-      <c r="AI1" t="s" s="7">
+      <c r="AE1" t="s" s="26">
         <v>40</v>
       </c>
-      <c r="AJ1" t="s" s="7">
+      <c r="AF1" t="s" s="26">
         <v>41</v>
       </c>
-      <c r="AK1" t="s" s="7">
+      <c r="AG1" t="s" s="26">
         <v>42</v>
       </c>
-      <c r="AL1" t="s" s="7">
+      <c r="AH1" t="s" s="26">
         <v>43</v>
       </c>
-      <c r="AM1" t="s" s="7">
+      <c r="AI1" t="s" s="26">
         <v>44</v>
       </c>
-      <c r="AN1" t="s" s="7">
+      <c r="AJ1" t="s" s="26">
         <v>45</v>
       </c>
-      <c r="AO1" t="s" s="7">
+      <c r="AK1" t="s" s="26">
         <v>46</v>
       </c>
-      <c r="AP1" t="s" s="7">
+      <c r="AL1" t="s" s="26">
         <v>47</v>
       </c>
-      <c r="AQ1" t="s" s="7">
+      <c r="AM1" t="s" s="26">
         <v>48</v>
       </c>
-      <c r="AR1" t="s" s="7">
+      <c r="AN1" t="s" s="26">
         <v>49</v>
       </c>
-      <c r="AS1" t="s" s="7">
+      <c r="AO1" t="s" s="26">
         <v>50</v>
       </c>
-      <c r="AT1" t="s" s="7">
+      <c r="AP1" t="s" s="26">
         <v>51</v>
       </c>
-      <c r="AU1" t="s" s="7">
+      <c r="AQ1" t="s" s="26">
         <v>52</v>
       </c>
-      <c r="AV1" t="s" s="7">
+      <c r="AR1" t="s" s="26">
         <v>53</v>
       </c>
-      <c r="AW1" t="s" s="7">
+      <c r="AS1" t="s" s="26">
         <v>54</v>
       </c>
-      <c r="AX1" t="s" s="7">
+      <c r="AT1" t="s" s="26">
         <v>55</v>
       </c>
-      <c r="AY1" t="s" s="7">
+      <c r="AU1" t="s" s="26">
         <v>56</v>
       </c>
-      <c r="AZ1" t="s" s="7">
+      <c r="AV1" t="s" s="26">
         <v>57</v>
       </c>
-      <c r="BA1" t="s" s="7">
+      <c r="AW1" t="s" s="26">
         <v>58</v>
       </c>
-      <c r="BB1" t="s" s="7">
+      <c r="AX1" t="s" s="26">
         <v>59</v>
       </c>
-      <c r="BC1" t="s" s="7">
+      <c r="AY1" t="s" s="26">
         <v>60</v>
       </c>
-      <c r="BD1" t="s" s="7">
+      <c r="AZ1" t="s" s="26">
         <v>61</v>
       </c>
-      <c r="BE1" t="s" s="7">
+      <c r="BA1" t="s" s="26">
         <v>62</v>
       </c>
-      <c r="BF1" t="s" s="7">
+      <c r="BB1" t="s" s="26">
         <v>63</v>
+      </c>
+      <c r="BC1" t="s" s="26">
+        <v>64</v>
+      </c>
+      <c r="BD1" t="s" s="26">
+        <v>65</v>
+      </c>
+      <c r="BE1" t="s" s="26">
+        <v>66</v>
+      </c>
+      <c r="BF1" t="s" s="26">
+        <v>67</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="7">
-        <v>64</v>
-      </c>
-      <c r="B2" t="s" s="7">
-        <v>65</v>
-      </c>
-      <c r="C2" t="s" s="7">
-        <v>66</v>
-      </c>
-      <c r="D2" t="s" s="7">
-        <v>67</v>
-      </c>
-      <c r="E2" t="s" s="7">
+      <c r="A2" t="s" s="26">
         <v>68</v>
       </c>
-      <c r="F2" t="s" s="7">
+      <c r="B2" t="s" s="26">
         <v>69</v>
       </c>
-      <c r="G2" t="s" s="7">
+      <c r="C2" t="s" s="26">
         <v>70</v>
       </c>
-      <c r="H2" t="s" s="7">
+      <c r="D2" t="s" s="26">
         <v>71</v>
       </c>
-      <c r="I2" t="s" s="7">
+      <c r="E2" t="s" s="26">
         <v>72</v>
       </c>
-      <c r="J2" t="s" s="7">
+      <c r="F2" t="s" s="26">
         <v>73</v>
       </c>
-      <c r="K2" t="s" s="7">
+      <c r="G2" t="s" s="26">
         <v>74</v>
       </c>
-      <c r="L2" t="s" s="7">
+      <c r="H2" t="s" s="26">
         <v>75</v>
       </c>
-      <c r="M2" t="s" s="7">
+      <c r="I2" t="s" s="26">
         <v>76</v>
       </c>
-      <c r="N2" t="s" s="7">
+      <c r="J2" t="s" s="26">
         <v>77</v>
       </c>
-      <c r="O2" t="s" s="7">
+      <c r="K2" t="s" s="26">
         <v>78</v>
       </c>
-      <c r="P2" t="s" s="7">
+      <c r="L2" t="s" s="26">
         <v>79</v>
       </c>
-      <c r="Q2" t="s" s="7">
+      <c r="M2" t="s" s="26">
         <v>80</v>
       </c>
-      <c r="R2" t="s" s="7">
+      <c r="N2" t="s" s="26">
         <v>81</v>
       </c>
-      <c r="S2" t="s" s="7">
+      <c r="O2" t="s" s="26">
         <v>82</v>
       </c>
-      <c r="T2" t="s" s="7">
+      <c r="P2" t="s" s="26">
         <v>83</v>
       </c>
-      <c r="U2" t="s" s="7">
+      <c r="Q2" t="s" s="26">
         <v>84</v>
       </c>
-      <c r="V2" t="s" s="7">
+      <c r="R2" t="s" s="26">
         <v>85</v>
       </c>
-      <c r="W2" t="s" s="7">
+      <c r="S2" t="s" s="26">
         <v>86</v>
       </c>
-      <c r="X2" t="s" s="7">
+      <c r="T2" t="s" s="26">
         <v>87</v>
       </c>
-      <c r="Y2" t="s" s="7">
+      <c r="U2" t="s" s="26">
         <v>88</v>
       </c>
-      <c r="Z2" t="s" s="7">
+      <c r="V2" t="s" s="26">
         <v>89</v>
       </c>
-      <c r="AA2" t="s" s="7">
+      <c r="W2" t="s" s="26">
         <v>90</v>
       </c>
-      <c r="AB2" t="s" s="7">
+      <c r="X2" t="s" s="26">
         <v>91</v>
       </c>
-      <c r="AC2" t="s" s="7">
+      <c r="Y2" t="s" s="26">
         <v>92</v>
       </c>
-      <c r="AD2" t="s" s="7">
+      <c r="Z2" t="s" s="26">
         <v>93</v>
       </c>
-      <c r="AE2" t="s" s="7">
+      <c r="AA2" t="s" s="26">
         <v>94</v>
       </c>
-      <c r="AF2" t="s" s="7">
+      <c r="AB2" t="s" s="26">
         <v>95</v>
       </c>
-      <c r="AG2" t="s" s="7">
+      <c r="AC2" t="s" s="26">
         <v>96</v>
       </c>
-      <c r="AH2" t="s" s="7">
+      <c r="AD2" t="s" s="26">
         <v>97</v>
       </c>
-      <c r="AI2" t="s" s="7">
+      <c r="AE2" t="s" s="26">
         <v>98</v>
       </c>
-      <c r="AJ2" t="s" s="7">
+      <c r="AF2" t="s" s="26">
         <v>99</v>
       </c>
-      <c r="AK2" t="s" s="7">
+      <c r="AG2" t="s" s="26">
         <v>100</v>
       </c>
-      <c r="AL2" t="s" s="7">
+      <c r="AH2" t="s" s="26">
         <v>101</v>
       </c>
-      <c r="AM2" t="s" s="7">
+      <c r="AI2" t="s" s="26">
         <v>102</v>
       </c>
-      <c r="AN2" t="s" s="7">
+      <c r="AJ2" t="s" s="26">
         <v>103</v>
       </c>
-      <c r="AO2" t="s" s="7">
+      <c r="AK2" t="s" s="26">
         <v>104</v>
       </c>
-      <c r="AP2" t="s" s="7">
+      <c r="AL2" t="s" s="26">
         <v>105</v>
       </c>
-      <c r="AQ2" t="s" s="7">
+      <c r="AM2" t="s" s="26">
         <v>106</v>
       </c>
-      <c r="AR2" t="s" s="7">
+      <c r="AN2" t="s" s="26">
         <v>107</v>
       </c>
-      <c r="AS2" t="s" s="7">
+      <c r="AO2" t="s" s="26">
         <v>108</v>
       </c>
-      <c r="AT2" t="s" s="7">
+      <c r="AP2" t="s" s="26">
         <v>109</v>
       </c>
-      <c r="AU2" t="s" s="7">
+      <c r="AQ2" t="s" s="26">
         <v>110</v>
       </c>
-      <c r="AV2" t="s" s="7">
+      <c r="AR2" t="s" s="26">
         <v>111</v>
       </c>
-      <c r="AW2" t="s" s="7">
+      <c r="AS2" t="s" s="26">
         <v>112</v>
       </c>
-      <c r="AX2" t="s" s="7">
+      <c r="AT2" t="s" s="26">
         <v>113</v>
       </c>
-      <c r="AY2" t="s" s="7">
+      <c r="AU2" t="s" s="26">
         <v>114</v>
       </c>
-      <c r="AZ2" t="s" s="7">
+      <c r="AV2" t="s" s="26">
         <v>115</v>
       </c>
-      <c r="BA2" t="s" s="7">
+      <c r="AW2" t="s" s="26">
         <v>116</v>
       </c>
-      <c r="BB2" t="s" s="7">
+      <c r="AX2" t="s" s="26">
         <v>117</v>
       </c>
-      <c r="BC2" t="s" s="7">
+      <c r="AY2" t="s" s="26">
         <v>118</v>
       </c>
-      <c r="BD2" t="s" s="7">
+      <c r="AZ2" t="s" s="26">
         <v>119</v>
       </c>
-      <c r="BE2" t="s" s="7">
+      <c r="BA2" t="s" s="26">
         <v>120</v>
       </c>
-      <c r="BF2" t="s" s="7">
+      <c r="BB2" t="s" s="26">
         <v>121</v>
+      </c>
+      <c r="BC2" t="s" s="26">
+        <v>122</v>
+      </c>
+      <c r="BD2" t="s" s="26">
+        <v>123</v>
+      </c>
+      <c r="BE2" t="s" s="26">
+        <v>124</v>
+      </c>
+      <c r="BF2" t="s" s="26">
+        <v>125</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="8">
+      <c r="A3" s="27">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="7">
-        <v>122</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" t="s" s="7">
-        <v>123</v>
-      </c>
-      <c r="E3" t="s" s="7">
-        <v>123</v>
-      </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" t="b" s="8">
-        <v>0</v>
-      </c>
-      <c r="L3" s="8">
+      <c r="B3" t="s" s="26">
+        <v>126</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" t="s" s="26">
+        <v>127</v>
+      </c>
+      <c r="E3" t="s" s="26">
+        <v>127</v>
+      </c>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" t="b" s="27">
+        <v>0</v>
+      </c>
+      <c r="L3" s="27">
         <v>1</v>
       </c>
-      <c r="M3" s="8">
-        <v>0</v>
-      </c>
-      <c r="N3" s="8">
-        <v>0</v>
-      </c>
-      <c r="O3" s="11">
-        <v>0</v>
-      </c>
-      <c r="P3" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="8">
+      <c r="M3" s="27">
+        <v>0</v>
+      </c>
+      <c r="N3" s="27">
+        <v>0</v>
+      </c>
+      <c r="O3" s="30">
+        <v>0</v>
+      </c>
+      <c r="P3" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="27">
         <v>1</v>
       </c>
-      <c r="R3" s="8">
-        <v>0</v>
-      </c>
-      <c r="S3" s="8">
-        <v>0</v>
-      </c>
-      <c r="T3" s="8">
-        <v>0</v>
-      </c>
-      <c r="U3" s="8">
-        <v>0</v>
-      </c>
-      <c r="V3" s="8">
-        <v>0</v>
-      </c>
-      <c r="W3" s="8">
-        <v>0</v>
-      </c>
-      <c r="X3" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="8">
+      <c r="R3" s="27">
+        <v>0</v>
+      </c>
+      <c r="S3" s="27">
+        <v>0</v>
+      </c>
+      <c r="T3" s="27">
+        <v>0</v>
+      </c>
+      <c r="U3" s="27">
+        <v>0</v>
+      </c>
+      <c r="V3" s="27">
+        <v>0</v>
+      </c>
+      <c r="W3" s="27">
+        <v>0</v>
+      </c>
+      <c r="X3" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="27">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="27">
         <v>1</v>
       </c>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="10"/>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="10"/>
-      <c r="AJ3" s="10"/>
-      <c r="AK3" s="10"/>
-      <c r="AL3" s="10"/>
-      <c r="AM3" s="10"/>
-      <c r="AN3" s="10"/>
-      <c r="AO3" s="10"/>
-      <c r="AP3" s="10"/>
-      <c r="AQ3" s="10"/>
-      <c r="AR3" s="10"/>
-      <c r="AS3" s="10"/>
-      <c r="AT3" s="10"/>
-      <c r="AU3" s="10"/>
-      <c r="AV3" s="10"/>
-      <c r="AW3" s="10"/>
-      <c r="AX3" s="10"/>
-      <c r="AY3" s="10"/>
-      <c r="AZ3" s="10"/>
-      <c r="BA3" s="10"/>
-      <c r="BB3" s="10"/>
-      <c r="BC3" s="10"/>
-      <c r="BD3" s="10"/>
-      <c r="BE3" s="10"/>
-      <c r="BF3" s="10"/>
+      <c r="AF3" s="29"/>
+      <c r="AG3" s="29"/>
+      <c r="AH3" s="29"/>
+      <c r="AI3" s="29"/>
+      <c r="AJ3" s="29"/>
+      <c r="AK3" s="29"/>
+      <c r="AL3" s="29"/>
+      <c r="AM3" s="29"/>
+      <c r="AN3" s="29"/>
+      <c r="AO3" s="29"/>
+      <c r="AP3" s="29"/>
+      <c r="AQ3" s="29"/>
+      <c r="AR3" s="29"/>
+      <c r="AS3" s="29"/>
+      <c r="AT3" s="29"/>
+      <c r="AU3" s="29"/>
+      <c r="AV3" s="29"/>
+      <c r="AW3" s="29"/>
+      <c r="AX3" s="29"/>
+      <c r="AY3" s="29"/>
+      <c r="AZ3" s="29"/>
+      <c r="BA3" s="29"/>
+      <c r="BB3" s="29"/>
+      <c r="BC3" s="29"/>
+      <c r="BD3" s="29"/>
+      <c r="BE3" s="29"/>
+      <c r="BF3" s="29"/>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="8">
+      <c r="A4" s="27">
         <v>2</v>
       </c>
-      <c r="B4" t="s" s="7">
-        <v>122</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" t="s" s="7">
-        <v>123</v>
-      </c>
-      <c r="E4" t="s" s="7">
-        <v>123</v>
-      </c>
-      <c r="F4" t="s" s="12">
-        <v>124</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="I4" t="s" s="7">
-        <v>125</v>
-      </c>
-      <c r="J4" s="10"/>
-      <c r="K4" t="b" s="8">
-        <v>0</v>
-      </c>
-      <c r="L4" s="8">
+      <c r="B4" t="s" s="26">
+        <v>126</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" t="s" s="26">
+        <v>127</v>
+      </c>
+      <c r="E4" t="s" s="26">
+        <v>127</v>
+      </c>
+      <c r="F4" t="s" s="31">
+        <v>128</v>
+      </c>
+      <c r="G4" s="28"/>
+      <c r="H4" s="29"/>
+      <c r="I4" t="s" s="26">
+        <v>129</v>
+      </c>
+      <c r="J4" s="29"/>
+      <c r="K4" t="b" s="27">
+        <v>0</v>
+      </c>
+      <c r="L4" s="27">
         <v>2</v>
       </c>
-      <c r="M4" s="8">
-        <v>0</v>
-      </c>
-      <c r="N4" s="8">
-        <v>0</v>
-      </c>
-      <c r="O4" s="8">
-        <v>0</v>
-      </c>
-      <c r="P4" s="8">
+      <c r="M4" s="27">
+        <v>0</v>
+      </c>
+      <c r="N4" s="27">
+        <v>0</v>
+      </c>
+      <c r="O4" s="27">
+        <v>0</v>
+      </c>
+      <c r="P4" s="27">
         <v>1</v>
       </c>
-      <c r="Q4" s="8">
+      <c r="Q4" s="27">
         <v>1</v>
       </c>
-      <c r="R4" s="8">
-        <v>0</v>
-      </c>
-      <c r="S4" s="8">
-        <v>0</v>
-      </c>
-      <c r="T4" s="8">
-        <v>0</v>
-      </c>
-      <c r="U4" s="8">
-        <v>0</v>
-      </c>
-      <c r="V4" s="8">
-        <v>0</v>
-      </c>
-      <c r="W4" s="8">
-        <v>0</v>
-      </c>
-      <c r="X4" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="8">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="8">
+      <c r="R4" s="27">
+        <v>0</v>
+      </c>
+      <c r="S4" s="27">
+        <v>0</v>
+      </c>
+      <c r="T4" s="27">
+        <v>0</v>
+      </c>
+      <c r="U4" s="27">
+        <v>0</v>
+      </c>
+      <c r="V4" s="27">
+        <v>0</v>
+      </c>
+      <c r="W4" s="27">
+        <v>0</v>
+      </c>
+      <c r="X4" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="27">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="27">
         <v>1</v>
       </c>
-      <c r="AF4" s="10"/>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="10"/>
-      <c r="AL4" s="10"/>
-      <c r="AM4" s="10"/>
-      <c r="AN4" s="10"/>
-      <c r="AO4" s="10"/>
-      <c r="AP4" s="10"/>
-      <c r="AQ4" s="10"/>
-      <c r="AR4" s="10"/>
-      <c r="AS4" s="10"/>
-      <c r="AT4" s="10"/>
-      <c r="AU4" s="10"/>
-      <c r="AV4" s="10"/>
-      <c r="AW4" s="10"/>
-      <c r="AX4" s="10"/>
-      <c r="AY4" s="10"/>
-      <c r="AZ4" s="10"/>
-      <c r="BA4" s="10"/>
-      <c r="BB4" s="10"/>
-      <c r="BC4" s="10"/>
-      <c r="BD4" s="10"/>
-      <c r="BE4" s="10"/>
-      <c r="BF4" s="10"/>
+      <c r="AF4" s="29"/>
+      <c r="AG4" s="29"/>
+      <c r="AH4" s="29"/>
+      <c r="AI4" s="29"/>
+      <c r="AJ4" s="29"/>
+      <c r="AK4" s="29"/>
+      <c r="AL4" s="29"/>
+      <c r="AM4" s="29"/>
+      <c r="AN4" s="29"/>
+      <c r="AO4" s="29"/>
+      <c r="AP4" s="29"/>
+      <c r="AQ4" s="29"/>
+      <c r="AR4" s="29"/>
+      <c r="AS4" s="29"/>
+      <c r="AT4" s="29"/>
+      <c r="AU4" s="29"/>
+      <c r="AV4" s="29"/>
+      <c r="AW4" s="29"/>
+      <c r="AX4" s="29"/>
+      <c r="AY4" s="29"/>
+      <c r="AZ4" s="29"/>
+      <c r="BA4" s="29"/>
+      <c r="BB4" s="29"/>
+      <c r="BC4" s="29"/>
+      <c r="BD4" s="29"/>
+      <c r="BE4" s="29"/>
+      <c r="BF4" s="29"/>
     </row>
     <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="8">
+      <c r="A5" s="27">
         <v>3</v>
       </c>
-      <c r="B5" t="s" s="7">
-        <v>122</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" t="s" s="7">
-        <v>123</v>
-      </c>
-      <c r="E5" t="s" s="7">
-        <v>123</v>
-      </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" t="b" s="8">
-        <v>0</v>
-      </c>
-      <c r="L5" s="8">
+      <c r="B5" t="s" s="26">
+        <v>126</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" t="s" s="26">
+        <v>127</v>
+      </c>
+      <c r="E5" t="s" s="26">
+        <v>127</v>
+      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" t="b" s="27">
+        <v>0</v>
+      </c>
+      <c r="L5" s="27">
         <v>3</v>
       </c>
-      <c r="M5" s="8">
-        <v>0</v>
-      </c>
-      <c r="N5" s="8">
-        <v>0</v>
-      </c>
-      <c r="O5" s="8">
-        <v>0</v>
-      </c>
-      <c r="P5" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="11">
+      <c r="M5" s="27">
+        <v>0</v>
+      </c>
+      <c r="N5" s="27">
+        <v>0</v>
+      </c>
+      <c r="O5" s="27">
+        <v>0</v>
+      </c>
+      <c r="P5" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="30">
         <v>2</v>
       </c>
-      <c r="R5" s="8">
-        <v>0</v>
-      </c>
-      <c r="S5" s="8">
-        <v>0</v>
-      </c>
-      <c r="T5" s="8">
-        <v>0</v>
-      </c>
-      <c r="U5" s="8">
-        <v>0</v>
-      </c>
-      <c r="V5" s="8">
+      <c r="R5" s="27">
+        <v>0</v>
+      </c>
+      <c r="S5" s="27">
+        <v>0</v>
+      </c>
+      <c r="T5" s="27">
+        <v>0</v>
+      </c>
+      <c r="U5" s="27">
+        <v>0</v>
+      </c>
+      <c r="V5" s="27">
         <v>1</v>
       </c>
-      <c r="W5" s="8">
-        <v>0</v>
-      </c>
-      <c r="X5" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="8">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="8">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="10"/>
-      <c r="AG5" s="10"/>
-      <c r="AH5" s="10"/>
-      <c r="AI5" s="10"/>
-      <c r="AJ5" s="10"/>
-      <c r="AK5" s="10"/>
-      <c r="AL5" s="10"/>
-      <c r="AM5" s="10"/>
-      <c r="AN5" s="10"/>
-      <c r="AO5" s="10"/>
-      <c r="AP5" s="10"/>
-      <c r="AQ5" s="10"/>
-      <c r="AR5" s="10"/>
-      <c r="AS5" s="10"/>
-      <c r="AT5" s="10"/>
-      <c r="AU5" s="10"/>
-      <c r="AV5" s="10"/>
-      <c r="AW5" s="10"/>
-      <c r="AX5" s="10"/>
-      <c r="AY5" s="10"/>
-      <c r="AZ5" s="10"/>
-      <c r="BA5" s="10"/>
-      <c r="BB5" s="10"/>
-      <c r="BC5" s="10"/>
-      <c r="BD5" s="10"/>
-      <c r="BE5" s="10"/>
-      <c r="BF5" s="10"/>
+      <c r="W5" s="27">
+        <v>0</v>
+      </c>
+      <c r="X5" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="27">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="27">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="29"/>
+      <c r="AG5" s="29"/>
+      <c r="AH5" s="29"/>
+      <c r="AI5" s="29"/>
+      <c r="AJ5" s="29"/>
+      <c r="AK5" s="29"/>
+      <c r="AL5" s="29"/>
+      <c r="AM5" s="29"/>
+      <c r="AN5" s="29"/>
+      <c r="AO5" s="29"/>
+      <c r="AP5" s="29"/>
+      <c r="AQ5" s="29"/>
+      <c r="AR5" s="29"/>
+      <c r="AS5" s="29"/>
+      <c r="AT5" s="29"/>
+      <c r="AU5" s="29"/>
+      <c r="AV5" s="29"/>
+      <c r="AW5" s="29"/>
+      <c r="AX5" s="29"/>
+      <c r="AY5" s="29"/>
+      <c r="AZ5" s="29"/>
+      <c r="BA5" s="29"/>
+      <c r="BB5" s="29"/>
+      <c r="BC5" s="29"/>
+      <c r="BD5" s="29"/>
+      <c r="BE5" s="29"/>
+      <c r="BF5" s="29"/>
     </row>
     <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="10"/>
-      <c r="AB6" s="10"/>
-      <c r="AC6" s="10"/>
-      <c r="AD6" s="10"/>
-      <c r="AE6" s="10"/>
-      <c r="AF6" s="10"/>
-      <c r="AG6" s="10"/>
-      <c r="AH6" s="10"/>
-      <c r="AI6" s="10"/>
-      <c r="AJ6" s="10"/>
-      <c r="AK6" s="10"/>
-      <c r="AL6" s="10"/>
-      <c r="AM6" s="10"/>
-      <c r="AN6" s="10"/>
-      <c r="AO6" s="10"/>
-      <c r="AP6" s="10"/>
-      <c r="AQ6" s="10"/>
-      <c r="AR6" s="10"/>
-      <c r="AS6" s="10"/>
-      <c r="AT6" s="10"/>
-      <c r="AU6" s="10"/>
-      <c r="AV6" s="10"/>
-      <c r="AW6" s="10"/>
-      <c r="AX6" s="10"/>
-      <c r="AY6" s="10"/>
-      <c r="AZ6" s="10"/>
-      <c r="BA6" s="10"/>
-      <c r="BB6" s="10"/>
-      <c r="BC6" s="10"/>
-      <c r="BD6" s="10"/>
-      <c r="BE6" s="10"/>
-      <c r="BF6" s="10"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="29"/>
+      <c r="X6" s="29"/>
+      <c r="Y6" s="29"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="29"/>
+      <c r="AB6" s="29"/>
+      <c r="AC6" s="29"/>
+      <c r="AD6" s="29"/>
+      <c r="AE6" s="29"/>
+      <c r="AF6" s="29"/>
+      <c r="AG6" s="29"/>
+      <c r="AH6" s="29"/>
+      <c r="AI6" s="29"/>
+      <c r="AJ6" s="29"/>
+      <c r="AK6" s="29"/>
+      <c r="AL6" s="29"/>
+      <c r="AM6" s="29"/>
+      <c r="AN6" s="29"/>
+      <c r="AO6" s="29"/>
+      <c r="AP6" s="29"/>
+      <c r="AQ6" s="29"/>
+      <c r="AR6" s="29"/>
+      <c r="AS6" s="29"/>
+      <c r="AT6" s="29"/>
+      <c r="AU6" s="29"/>
+      <c r="AV6" s="29"/>
+      <c r="AW6" s="29"/>
+      <c r="AX6" s="29"/>
+      <c r="AY6" s="29"/>
+      <c r="AZ6" s="29"/>
+      <c r="BA6" s="29"/>
+      <c r="BB6" s="29"/>
+      <c r="BC6" s="29"/>
+      <c r="BD6" s="29"/>
+      <c r="BE6" s="29"/>
+      <c r="BF6" s="29"/>
     </row>
     <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="10"/>
-      <c r="Z7" s="10"/>
-      <c r="AA7" s="10"/>
-      <c r="AB7" s="10"/>
-      <c r="AC7" s="10"/>
-      <c r="AD7" s="10"/>
-      <c r="AE7" s="10"/>
-      <c r="AF7" s="10"/>
-      <c r="AG7" s="10"/>
-      <c r="AH7" s="10"/>
-      <c r="AI7" s="10"/>
-      <c r="AJ7" s="10"/>
-      <c r="AK7" s="10"/>
-      <c r="AL7" s="10"/>
-      <c r="AM7" s="10"/>
-      <c r="AN7" s="10"/>
-      <c r="AO7" s="10"/>
-      <c r="AP7" s="10"/>
-      <c r="AQ7" s="10"/>
-      <c r="AR7" s="10"/>
-      <c r="AS7" s="10"/>
-      <c r="AT7" s="10"/>
-      <c r="AU7" s="10"/>
-      <c r="AV7" s="10"/>
-      <c r="AW7" s="10"/>
-      <c r="AX7" s="10"/>
-      <c r="AY7" s="10"/>
-      <c r="AZ7" s="10"/>
-      <c r="BA7" s="10"/>
-      <c r="BB7" s="10"/>
-      <c r="BC7" s="10"/>
-      <c r="BD7" s="10"/>
-      <c r="BE7" s="10"/>
-      <c r="BF7" s="10"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="29"/>
+      <c r="AB7" s="29"/>
+      <c r="AC7" s="29"/>
+      <c r="AD7" s="29"/>
+      <c r="AE7" s="29"/>
+      <c r="AF7" s="29"/>
+      <c r="AG7" s="29"/>
+      <c r="AH7" s="29"/>
+      <c r="AI7" s="29"/>
+      <c r="AJ7" s="29"/>
+      <c r="AK7" s="29"/>
+      <c r="AL7" s="29"/>
+      <c r="AM7" s="29"/>
+      <c r="AN7" s="29"/>
+      <c r="AO7" s="29"/>
+      <c r="AP7" s="29"/>
+      <c r="AQ7" s="29"/>
+      <c r="AR7" s="29"/>
+      <c r="AS7" s="29"/>
+      <c r="AT7" s="29"/>
+      <c r="AU7" s="29"/>
+      <c r="AV7" s="29"/>
+      <c r="AW7" s="29"/>
+      <c r="AX7" s="29"/>
+      <c r="AY7" s="29"/>
+      <c r="AZ7" s="29"/>
+      <c r="BA7" s="29"/>
+      <c r="BB7" s="29"/>
+      <c r="BC7" s="29"/>
+      <c r="BD7" s="29"/>
+      <c r="BE7" s="29"/>
+      <c r="BF7" s="29"/>
     </row>
     <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="10"/>
-      <c r="AA8" s="10"/>
-      <c r="AB8" s="10"/>
-      <c r="AC8" s="10"/>
-      <c r="AD8" s="10"/>
-      <c r="AE8" s="10"/>
-      <c r="AF8" s="10"/>
-      <c r="AG8" s="10"/>
-      <c r="AH8" s="10"/>
-      <c r="AI8" s="10"/>
-      <c r="AJ8" s="10"/>
-      <c r="AK8" s="10"/>
-      <c r="AL8" s="10"/>
-      <c r="AM8" s="10"/>
-      <c r="AN8" s="10"/>
-      <c r="AO8" s="10"/>
-      <c r="AP8" s="10"/>
-      <c r="AQ8" s="10"/>
-      <c r="AR8" s="10"/>
-      <c r="AS8" s="10"/>
-      <c r="AT8" s="10"/>
-      <c r="AU8" s="10"/>
-      <c r="AV8" s="10"/>
-      <c r="AW8" s="10"/>
-      <c r="AX8" s="10"/>
-      <c r="AY8" s="10"/>
-      <c r="AZ8" s="10"/>
-      <c r="BA8" s="10"/>
-      <c r="BB8" s="10"/>
-      <c r="BC8" s="10"/>
-      <c r="BD8" s="10"/>
-      <c r="BE8" s="10"/>
-      <c r="BF8" s="10"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="29"/>
+      <c r="V8" s="29"/>
+      <c r="W8" s="29"/>
+      <c r="X8" s="29"/>
+      <c r="Y8" s="29"/>
+      <c r="Z8" s="29"/>
+      <c r="AA8" s="29"/>
+      <c r="AB8" s="29"/>
+      <c r="AC8" s="29"/>
+      <c r="AD8" s="29"/>
+      <c r="AE8" s="29"/>
+      <c r="AF8" s="29"/>
+      <c r="AG8" s="29"/>
+      <c r="AH8" s="29"/>
+      <c r="AI8" s="29"/>
+      <c r="AJ8" s="29"/>
+      <c r="AK8" s="29"/>
+      <c r="AL8" s="29"/>
+      <c r="AM8" s="29"/>
+      <c r="AN8" s="29"/>
+      <c r="AO8" s="29"/>
+      <c r="AP8" s="29"/>
+      <c r="AQ8" s="29"/>
+      <c r="AR8" s="29"/>
+      <c r="AS8" s="29"/>
+      <c r="AT8" s="29"/>
+      <c r="AU8" s="29"/>
+      <c r="AV8" s="29"/>
+      <c r="AW8" s="29"/>
+      <c r="AX8" s="29"/>
+      <c r="AY8" s="29"/>
+      <c r="AZ8" s="29"/>
+      <c r="BA8" s="29"/>
+      <c r="BB8" s="29"/>
+      <c r="BC8" s="29"/>
+      <c r="BD8" s="29"/>
+      <c r="BE8" s="29"/>
+      <c r="BF8" s="29"/>
     </row>
     <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="10"/>
-      <c r="AA9" s="10"/>
-      <c r="AB9" s="10"/>
-      <c r="AC9" s="10"/>
-      <c r="AD9" s="10"/>
-      <c r="AE9" s="10"/>
-      <c r="AF9" s="10"/>
-      <c r="AG9" s="10"/>
-      <c r="AH9" s="10"/>
-      <c r="AI9" s="10"/>
-      <c r="AJ9" s="10"/>
-      <c r="AK9" s="10"/>
-      <c r="AL9" s="10"/>
-      <c r="AM9" s="10"/>
-      <c r="AN9" s="10"/>
-      <c r="AO9" s="10"/>
-      <c r="AP9" s="10"/>
-      <c r="AQ9" s="10"/>
-      <c r="AR9" s="10"/>
-      <c r="AS9" s="10"/>
-      <c r="AT9" s="10"/>
-      <c r="AU9" s="10"/>
-      <c r="AV9" s="10"/>
-      <c r="AW9" s="10"/>
-      <c r="AX9" s="10"/>
-      <c r="AY9" s="10"/>
-      <c r="AZ9" s="10"/>
-      <c r="BA9" s="10"/>
-      <c r="BB9" s="10"/>
-      <c r="BC9" s="10"/>
-      <c r="BD9" s="10"/>
-      <c r="BE9" s="10"/>
-      <c r="BF9" s="10"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="29"/>
+      <c r="X9" s="29"/>
+      <c r="Y9" s="29"/>
+      <c r="Z9" s="29"/>
+      <c r="AA9" s="29"/>
+      <c r="AB9" s="29"/>
+      <c r="AC9" s="29"/>
+      <c r="AD9" s="29"/>
+      <c r="AE9" s="29"/>
+      <c r="AF9" s="29"/>
+      <c r="AG9" s="29"/>
+      <c r="AH9" s="29"/>
+      <c r="AI9" s="29"/>
+      <c r="AJ9" s="29"/>
+      <c r="AK9" s="29"/>
+      <c r="AL9" s="29"/>
+      <c r="AM9" s="29"/>
+      <c r="AN9" s="29"/>
+      <c r="AO9" s="29"/>
+      <c r="AP9" s="29"/>
+      <c r="AQ9" s="29"/>
+      <c r="AR9" s="29"/>
+      <c r="AS9" s="29"/>
+      <c r="AT9" s="29"/>
+      <c r="AU9" s="29"/>
+      <c r="AV9" s="29"/>
+      <c r="AW9" s="29"/>
+      <c r="AX9" s="29"/>
+      <c r="AY9" s="29"/>
+      <c r="AZ9" s="29"/>
+      <c r="BA9" s="29"/>
+      <c r="BB9" s="29"/>
+      <c r="BC9" s="29"/>
+      <c r="BD9" s="29"/>
+      <c r="BE9" s="29"/>
+      <c r="BF9" s="29"/>
     </row>
     <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="10"/>
-      <c r="AA10" s="10"/>
-      <c r="AB10" s="10"/>
-      <c r="AC10" s="10"/>
-      <c r="AD10" s="10"/>
-      <c r="AE10" s="10"/>
-      <c r="AF10" s="10"/>
-      <c r="AG10" s="10"/>
-      <c r="AH10" s="10"/>
-      <c r="AI10" s="10"/>
-      <c r="AJ10" s="10"/>
-      <c r="AK10" s="10"/>
-      <c r="AL10" s="10"/>
-      <c r="AM10" s="10"/>
-      <c r="AN10" s="10"/>
-      <c r="AO10" s="10"/>
-      <c r="AP10" s="10"/>
-      <c r="AQ10" s="10"/>
-      <c r="AR10" s="10"/>
-      <c r="AS10" s="10"/>
-      <c r="AT10" s="10"/>
-      <c r="AU10" s="10"/>
-      <c r="AV10" s="10"/>
-      <c r="AW10" s="10"/>
-      <c r="AX10" s="10"/>
-      <c r="AY10" s="10"/>
-      <c r="AZ10" s="10"/>
-      <c r="BA10" s="10"/>
-      <c r="BB10" s="10"/>
-      <c r="BC10" s="10"/>
-      <c r="BD10" s="10"/>
-      <c r="BE10" s="10"/>
-      <c r="BF10" s="10"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="29"/>
+      <c r="W10" s="29"/>
+      <c r="X10" s="29"/>
+      <c r="Y10" s="29"/>
+      <c r="Z10" s="29"/>
+      <c r="AA10" s="29"/>
+      <c r="AB10" s="29"/>
+      <c r="AC10" s="29"/>
+      <c r="AD10" s="29"/>
+      <c r="AE10" s="29"/>
+      <c r="AF10" s="29"/>
+      <c r="AG10" s="29"/>
+      <c r="AH10" s="29"/>
+      <c r="AI10" s="29"/>
+      <c r="AJ10" s="29"/>
+      <c r="AK10" s="29"/>
+      <c r="AL10" s="29"/>
+      <c r="AM10" s="29"/>
+      <c r="AN10" s="29"/>
+      <c r="AO10" s="29"/>
+      <c r="AP10" s="29"/>
+      <c r="AQ10" s="29"/>
+      <c r="AR10" s="29"/>
+      <c r="AS10" s="29"/>
+      <c r="AT10" s="29"/>
+      <c r="AU10" s="29"/>
+      <c r="AV10" s="29"/>
+      <c r="AW10" s="29"/>
+      <c r="AX10" s="29"/>
+      <c r="AY10" s="29"/>
+      <c r="AZ10" s="29"/>
+      <c r="BA10" s="29"/>
+      <c r="BB10" s="29"/>
+      <c r="BC10" s="29"/>
+      <c r="BD10" s="29"/>
+      <c r="BE10" s="29"/>
+      <c r="BF10" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -3224,840 +3503,840 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.8516" style="13" customWidth="1"/>
-    <col min="2" max="2" width="12.6719" style="13" customWidth="1"/>
-    <col min="3" max="3" width="33.8516" style="13" customWidth="1"/>
-    <col min="4" max="4" width="7.85156" style="13" customWidth="1"/>
-    <col min="5" max="5" width="15.8516" style="13" customWidth="1"/>
-    <col min="6" max="6" width="12.8516" style="13" customWidth="1"/>
-    <col min="7" max="7" width="14" style="13" customWidth="1"/>
-    <col min="8" max="8" width="13.3516" style="13" customWidth="1"/>
-    <col min="9" max="9" width="11" style="13" customWidth="1"/>
-    <col min="10" max="10" width="15.8516" style="13" customWidth="1"/>
-    <col min="11" max="11" width="19.8516" style="13" customWidth="1"/>
-    <col min="12" max="12" width="8.35156" style="13" customWidth="1"/>
-    <col min="13" max="13" width="18.8516" style="13" customWidth="1"/>
-    <col min="14" max="14" width="11.8516" style="13" customWidth="1"/>
-    <col min="15" max="15" width="20.3516" style="13" customWidth="1"/>
-    <col min="16" max="16" width="18.3516" style="13" customWidth="1"/>
-    <col min="17" max="17" width="20.8516" style="13" customWidth="1"/>
-    <col min="18" max="18" width="18.1719" style="13" customWidth="1"/>
-    <col min="19" max="19" width="20" style="13" customWidth="1"/>
-    <col min="20" max="20" width="17.1719" style="13" customWidth="1"/>
-    <col min="21" max="21" width="19.5" style="13" customWidth="1"/>
-    <col min="22" max="22" width="14.5" style="13" customWidth="1"/>
-    <col min="23" max="23" width="15.6719" style="13" customWidth="1"/>
-    <col min="24" max="24" width="20" style="13" customWidth="1"/>
-    <col min="25" max="25" width="22.3516" style="13" customWidth="1"/>
-    <col min="26" max="26" width="17.3516" style="13" customWidth="1"/>
-    <col min="27" max="27" width="15.8516" style="13" customWidth="1"/>
-    <col min="28" max="28" width="14.3516" style="13" customWidth="1"/>
-    <col min="29" max="29" width="13" style="13" customWidth="1"/>
-    <col min="30" max="30" width="8.17188" style="13" customWidth="1"/>
-    <col min="31" max="31" width="37.5" style="13" customWidth="1"/>
-    <col min="32" max="32" width="14.1719" style="13" customWidth="1"/>
-    <col min="33" max="33" width="31.3516" style="13" customWidth="1"/>
-    <col min="34" max="34" width="39.1719" style="13" customWidth="1"/>
-    <col min="35" max="35" width="40" style="13" customWidth="1"/>
-    <col min="36" max="36" width="52.6719" style="13" customWidth="1"/>
-    <col min="37" max="37" width="56.8516" style="13" customWidth="1"/>
-    <col min="38" max="38" width="54.1719" style="13" customWidth="1"/>
-    <col min="39" max="39" width="45.6719" style="13" customWidth="1"/>
-    <col min="40" max="40" width="35.3516" style="13" customWidth="1"/>
-    <col min="41" max="41" width="32.8516" style="13" customWidth="1"/>
-    <col min="42" max="42" width="46.8516" style="13" customWidth="1"/>
-    <col min="43" max="43" width="45.1719" style="13" customWidth="1"/>
-    <col min="44" max="44" width="16.3516" style="13" customWidth="1"/>
-    <col min="45" max="45" width="34.3516" style="13" customWidth="1"/>
-    <col min="46" max="46" width="60.3516" style="13" customWidth="1"/>
-    <col min="47" max="16384" width="12.6719" style="13" customWidth="1"/>
+    <col min="1" max="1" width="10.8516" style="32" customWidth="1"/>
+    <col min="2" max="2" width="12.6719" style="32" customWidth="1"/>
+    <col min="3" max="3" width="33.8516" style="32" customWidth="1"/>
+    <col min="4" max="4" width="7.85156" style="32" customWidth="1"/>
+    <col min="5" max="5" width="15.8516" style="32" customWidth="1"/>
+    <col min="6" max="6" width="12.8516" style="32" customWidth="1"/>
+    <col min="7" max="7" width="14" style="32" customWidth="1"/>
+    <col min="8" max="8" width="13.3516" style="32" customWidth="1"/>
+    <col min="9" max="9" width="11" style="32" customWidth="1"/>
+    <col min="10" max="10" width="15.8516" style="32" customWidth="1"/>
+    <col min="11" max="11" width="19.8516" style="32" customWidth="1"/>
+    <col min="12" max="12" width="8.35156" style="32" customWidth="1"/>
+    <col min="13" max="13" width="18.8516" style="32" customWidth="1"/>
+    <col min="14" max="14" width="11.8516" style="32" customWidth="1"/>
+    <col min="15" max="15" width="20.3516" style="32" customWidth="1"/>
+    <col min="16" max="16" width="18.3516" style="32" customWidth="1"/>
+    <col min="17" max="17" width="20.8516" style="32" customWidth="1"/>
+    <col min="18" max="18" width="18.1719" style="32" customWidth="1"/>
+    <col min="19" max="19" width="20" style="32" customWidth="1"/>
+    <col min="20" max="20" width="17.1719" style="32" customWidth="1"/>
+    <col min="21" max="21" width="19.5" style="32" customWidth="1"/>
+    <col min="22" max="22" width="14.5" style="32" customWidth="1"/>
+    <col min="23" max="23" width="15.6719" style="32" customWidth="1"/>
+    <col min="24" max="24" width="20" style="32" customWidth="1"/>
+    <col min="25" max="25" width="22.3516" style="32" customWidth="1"/>
+    <col min="26" max="26" width="17.3516" style="32" customWidth="1"/>
+    <col min="27" max="27" width="15.8516" style="32" customWidth="1"/>
+    <col min="28" max="28" width="14.3516" style="32" customWidth="1"/>
+    <col min="29" max="29" width="13" style="32" customWidth="1"/>
+    <col min="30" max="30" width="8.17188" style="32" customWidth="1"/>
+    <col min="31" max="31" width="37.5" style="32" customWidth="1"/>
+    <col min="32" max="32" width="14.1719" style="32" customWidth="1"/>
+    <col min="33" max="33" width="31.3516" style="32" customWidth="1"/>
+    <col min="34" max="34" width="39.1719" style="32" customWidth="1"/>
+    <col min="35" max="35" width="40" style="32" customWidth="1"/>
+    <col min="36" max="36" width="52.6719" style="32" customWidth="1"/>
+    <col min="37" max="37" width="56.8516" style="32" customWidth="1"/>
+    <col min="38" max="38" width="54.1719" style="32" customWidth="1"/>
+    <col min="39" max="39" width="45.6719" style="32" customWidth="1"/>
+    <col min="40" max="40" width="35.3516" style="32" customWidth="1"/>
+    <col min="41" max="41" width="32.8516" style="32" customWidth="1"/>
+    <col min="42" max="42" width="46.8516" style="32" customWidth="1"/>
+    <col min="43" max="43" width="45.1719" style="32" customWidth="1"/>
+    <col min="44" max="44" width="16.3516" style="32" customWidth="1"/>
+    <col min="45" max="45" width="34.3516" style="32" customWidth="1"/>
+    <col min="46" max="46" width="60.3516" style="32" customWidth="1"/>
+    <col min="47" max="16384" width="12.6719" style="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="7">
-        <v>127</v>
-      </c>
-      <c r="C1" t="s" s="7">
-        <v>128</v>
-      </c>
-      <c r="D1" t="s" s="7">
-        <v>129</v>
-      </c>
-      <c r="E1" t="s" s="7">
+      <c r="A1" t="s" s="26">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s" s="26">
         <v>130</v>
       </c>
-      <c r="F1" t="s" s="7">
+      <c r="C1" t="s" s="26">
         <v>131</v>
       </c>
-      <c r="G1" t="s" s="7">
+      <c r="D1" t="s" s="26">
         <v>132</v>
       </c>
-      <c r="H1" t="s" s="7">
+      <c r="E1" t="s" s="26">
         <v>133</v>
       </c>
-      <c r="I1" t="s" s="7">
+      <c r="F1" t="s" s="26">
         <v>134</v>
       </c>
-      <c r="J1" t="s" s="7">
+      <c r="G1" t="s" s="26">
         <v>135</v>
       </c>
-      <c r="K1" t="s" s="7">
+      <c r="H1" t="s" s="26">
         <v>136</v>
       </c>
-      <c r="L1" t="s" s="7">
+      <c r="I1" t="s" s="26">
         <v>137</v>
       </c>
-      <c r="M1" t="s" s="7">
+      <c r="J1" t="s" s="26">
         <v>138</v>
       </c>
-      <c r="N1" t="s" s="7">
+      <c r="K1" t="s" s="26">
         <v>139</v>
       </c>
-      <c r="O1" t="s" s="7">
+      <c r="L1" t="s" s="26">
         <v>140</v>
       </c>
-      <c r="P1" t="s" s="7">
+      <c r="M1" t="s" s="26">
         <v>141</v>
       </c>
-      <c r="Q1" t="s" s="7">
+      <c r="N1" t="s" s="26">
         <v>142</v>
       </c>
-      <c r="R1" t="s" s="7">
+      <c r="O1" t="s" s="26">
         <v>143</v>
       </c>
-      <c r="S1" t="s" s="7">
+      <c r="P1" t="s" s="26">
         <v>144</v>
       </c>
-      <c r="T1" t="s" s="7">
+      <c r="Q1" t="s" s="26">
         <v>145</v>
       </c>
-      <c r="U1" t="s" s="7">
+      <c r="R1" t="s" s="26">
         <v>146</v>
       </c>
-      <c r="V1" t="s" s="7">
+      <c r="S1" t="s" s="26">
         <v>147</v>
       </c>
-      <c r="W1" t="s" s="7">
+      <c r="T1" t="s" s="26">
         <v>148</v>
       </c>
-      <c r="X1" t="s" s="7">
+      <c r="U1" t="s" s="26">
         <v>149</v>
       </c>
-      <c r="Y1" t="s" s="7">
+      <c r="V1" t="s" s="26">
         <v>150</v>
       </c>
-      <c r="Z1" t="s" s="7">
+      <c r="W1" t="s" s="26">
         <v>151</v>
       </c>
-      <c r="AA1" t="s" s="7">
+      <c r="X1" t="s" s="26">
         <v>152</v>
       </c>
-      <c r="AB1" t="s" s="7">
+      <c r="Y1" t="s" s="26">
         <v>153</v>
       </c>
-      <c r="AC1" t="s" s="7">
+      <c r="Z1" t="s" s="26">
         <v>154</v>
       </c>
-      <c r="AD1" t="s" s="7">
+      <c r="AA1" t="s" s="26">
         <v>155</v>
       </c>
-      <c r="AE1" t="s" s="7">
+      <c r="AB1" t="s" s="26">
         <v>156</v>
       </c>
-      <c r="AF1" t="s" s="7">
+      <c r="AC1" t="s" s="26">
         <v>157</v>
       </c>
-      <c r="AG1" t="s" s="7">
+      <c r="AD1" t="s" s="26">
         <v>158</v>
       </c>
-      <c r="AH1" t="s" s="7">
+      <c r="AE1" t="s" s="26">
         <v>159</v>
       </c>
-      <c r="AI1" t="s" s="7">
+      <c r="AF1" t="s" s="26">
         <v>160</v>
       </c>
-      <c r="AJ1" t="s" s="7">
+      <c r="AG1" t="s" s="26">
         <v>161</v>
       </c>
-      <c r="AK1" t="s" s="7">
+      <c r="AH1" t="s" s="26">
         <v>162</v>
       </c>
-      <c r="AL1" t="s" s="7">
+      <c r="AI1" t="s" s="26">
         <v>163</v>
       </c>
-      <c r="AM1" t="s" s="7">
+      <c r="AJ1" t="s" s="26">
         <v>164</v>
       </c>
-      <c r="AN1" t="s" s="7">
+      <c r="AK1" t="s" s="26">
         <v>165</v>
       </c>
-      <c r="AO1" t="s" s="7">
+      <c r="AL1" t="s" s="26">
         <v>166</v>
       </c>
-      <c r="AP1" t="s" s="7">
+      <c r="AM1" t="s" s="26">
         <v>167</v>
       </c>
-      <c r="AQ1" t="s" s="7">
+      <c r="AN1" t="s" s="26">
         <v>168</v>
       </c>
-      <c r="AR1" t="s" s="7">
+      <c r="AO1" t="s" s="26">
         <v>169</v>
       </c>
-      <c r="AS1" t="s" s="7">
+      <c r="AP1" t="s" s="26">
         <v>170</v>
       </c>
-      <c r="AT1" t="s" s="7">
+      <c r="AQ1" t="s" s="26">
         <v>171</v>
+      </c>
+      <c r="AR1" t="s" s="26">
+        <v>172</v>
+      </c>
+      <c r="AS1" t="s" s="26">
+        <v>173</v>
+      </c>
+      <c r="AT1" t="s" s="26">
+        <v>174</v>
       </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="7">
-        <v>64</v>
-      </c>
-      <c r="B2" t="s" s="7">
-        <v>172</v>
-      </c>
-      <c r="C2" t="s" s="7">
-        <v>173</v>
-      </c>
-      <c r="D2" t="s" s="7">
-        <v>174</v>
-      </c>
-      <c r="E2" t="s" s="7">
+      <c r="A2" t="s" s="26">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s" s="26">
         <v>175</v>
       </c>
-      <c r="F2" t="s" s="7">
+      <c r="C2" t="s" s="26">
         <v>176</v>
       </c>
-      <c r="G2" t="s" s="7">
+      <c r="D2" t="s" s="26">
         <v>177</v>
       </c>
-      <c r="H2" t="s" s="7">
+      <c r="E2" t="s" s="26">
         <v>178</v>
       </c>
-      <c r="I2" t="s" s="7">
+      <c r="F2" t="s" s="26">
         <v>179</v>
       </c>
-      <c r="J2" t="s" s="7">
+      <c r="G2" t="s" s="26">
         <v>180</v>
       </c>
-      <c r="K2" t="s" s="7">
+      <c r="H2" t="s" s="26">
         <v>181</v>
       </c>
-      <c r="L2" t="s" s="7">
+      <c r="I2" t="s" s="26">
         <v>182</v>
       </c>
-      <c r="M2" t="s" s="7">
+      <c r="J2" t="s" s="26">
         <v>183</v>
       </c>
-      <c r="N2" t="s" s="7">
+      <c r="K2" t="s" s="26">
         <v>184</v>
       </c>
-      <c r="O2" t="s" s="7">
+      <c r="L2" t="s" s="26">
         <v>185</v>
       </c>
-      <c r="P2" t="s" s="7">
+      <c r="M2" t="s" s="26">
         <v>186</v>
       </c>
-      <c r="Q2" t="s" s="7">
+      <c r="N2" t="s" s="26">
         <v>187</v>
       </c>
-      <c r="R2" t="s" s="7">
+      <c r="O2" t="s" s="26">
         <v>188</v>
       </c>
-      <c r="S2" t="s" s="7">
+      <c r="P2" t="s" s="26">
         <v>189</v>
       </c>
-      <c r="T2" t="s" s="7">
+      <c r="Q2" t="s" s="26">
         <v>190</v>
       </c>
-      <c r="U2" t="s" s="7">
+      <c r="R2" t="s" s="26">
         <v>191</v>
       </c>
-      <c r="V2" t="s" s="7">
+      <c r="S2" t="s" s="26">
         <v>192</v>
       </c>
-      <c r="W2" t="s" s="7">
+      <c r="T2" t="s" s="26">
         <v>193</v>
       </c>
-      <c r="X2" t="s" s="7">
+      <c r="U2" t="s" s="26">
         <v>194</v>
       </c>
-      <c r="Y2" t="s" s="7">
+      <c r="V2" t="s" s="26">
         <v>195</v>
       </c>
-      <c r="Z2" t="s" s="7">
+      <c r="W2" t="s" s="26">
         <v>196</v>
       </c>
-      <c r="AA2" t="s" s="7">
+      <c r="X2" t="s" s="26">
         <v>197</v>
       </c>
-      <c r="AB2" t="s" s="7">
+      <c r="Y2" t="s" s="26">
         <v>198</v>
       </c>
-      <c r="AC2" t="s" s="7">
+      <c r="Z2" t="s" s="26">
         <v>199</v>
       </c>
-      <c r="AD2" t="s" s="7">
-        <v>182</v>
-      </c>
-      <c r="AE2" t="s" s="7">
+      <c r="AA2" t="s" s="26">
         <v>200</v>
       </c>
-      <c r="AF2" t="s" s="7">
-        <v>99</v>
-      </c>
-      <c r="AG2" t="s" s="7">
+      <c r="AB2" t="s" s="26">
         <v>201</v>
       </c>
-      <c r="AH2" t="s" s="7">
+      <c r="AC2" t="s" s="26">
         <v>202</v>
       </c>
-      <c r="AI2" t="s" s="7">
+      <c r="AD2" t="s" s="26">
+        <v>185</v>
+      </c>
+      <c r="AE2" t="s" s="26">
         <v>203</v>
       </c>
-      <c r="AJ2" t="s" s="7">
+      <c r="AF2" t="s" s="26">
+        <v>103</v>
+      </c>
+      <c r="AG2" t="s" s="26">
         <v>204</v>
       </c>
-      <c r="AK2" t="s" s="7">
+      <c r="AH2" t="s" s="26">
         <v>205</v>
       </c>
-      <c r="AL2" t="s" s="7">
+      <c r="AI2" t="s" s="26">
         <v>206</v>
       </c>
-      <c r="AM2" t="s" s="7">
+      <c r="AJ2" t="s" s="26">
         <v>207</v>
       </c>
-      <c r="AN2" t="s" s="7">
+      <c r="AK2" t="s" s="26">
         <v>208</v>
       </c>
-      <c r="AO2" t="s" s="7">
+      <c r="AL2" t="s" s="26">
         <v>209</v>
       </c>
-      <c r="AP2" t="s" s="7">
+      <c r="AM2" t="s" s="26">
         <v>210</v>
       </c>
-      <c r="AQ2" t="s" s="7">
+      <c r="AN2" t="s" s="26">
         <v>211</v>
       </c>
-      <c r="AR2" t="s" s="7">
+      <c r="AO2" t="s" s="26">
         <v>212</v>
       </c>
-      <c r="AS2" t="s" s="7">
+      <c r="AP2" t="s" s="26">
         <v>213</v>
       </c>
-      <c r="AT2" t="s" s="7">
+      <c r="AQ2" t="s" s="26">
         <v>214</v>
+      </c>
+      <c r="AR2" t="s" s="26">
+        <v>215</v>
+      </c>
+      <c r="AS2" t="s" s="26">
+        <v>216</v>
+      </c>
+      <c r="AT2" t="s" s="26">
+        <v>217</v>
       </c>
     </row>
     <row r="3" ht="14.6" customHeight="1">
-      <c r="A3" s="8">
+      <c r="A3" s="27">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" t="s" s="7">
-        <v>215</v>
-      </c>
-      <c r="D3" t="s" s="7">
-        <v>216</v>
-      </c>
-      <c r="E3" t="s" s="12">
-        <v>217</v>
-      </c>
-      <c r="F3" t="s" s="7">
+      <c r="B3" s="29"/>
+      <c r="C3" t="s" s="26">
         <v>218</v>
       </c>
-      <c r="G3" t="s" s="7">
+      <c r="D3" t="s" s="26">
         <v>219</v>
       </c>
-      <c r="H3" t="s" s="7">
+      <c r="E3" t="s" s="31">
         <v>220</v>
       </c>
-      <c r="I3" t="s" s="7">
+      <c r="F3" t="s" s="26">
         <v>221</v>
       </c>
-      <c r="J3" s="14">
+      <c r="G3" t="s" s="26">
+        <v>222</v>
+      </c>
+      <c r="H3" t="s" s="26">
+        <v>223</v>
+      </c>
+      <c r="I3" t="s" s="26">
+        <v>224</v>
+      </c>
+      <c r="J3" s="33">
         <v>23045</v>
       </c>
-      <c r="K3" t="b" s="8">
-        <v>0</v>
-      </c>
-      <c r="L3" s="10"/>
-      <c r="M3" t="s" s="7">
-        <v>222</v>
-      </c>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="10"/>
-      <c r="AD3" s="10"/>
-      <c r="AE3" s="10"/>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="10"/>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="10"/>
-      <c r="AJ3" s="10"/>
-      <c r="AK3" s="10"/>
-      <c r="AL3" s="10"/>
-      <c r="AM3" s="10"/>
-      <c r="AN3" s="10"/>
-      <c r="AO3" s="10"/>
-      <c r="AP3" s="10"/>
-      <c r="AQ3" s="10"/>
-      <c r="AR3" s="10"/>
-      <c r="AS3" s="10"/>
-      <c r="AT3" s="10"/>
+      <c r="K3" t="b" s="27">
+        <v>0</v>
+      </c>
+      <c r="L3" s="29"/>
+      <c r="M3" t="s" s="26">
+        <v>225</v>
+      </c>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="29"/>
+      <c r="W3" s="29"/>
+      <c r="X3" s="29"/>
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="29"/>
+      <c r="AB3" s="29"/>
+      <c r="AC3" s="29"/>
+      <c r="AD3" s="29"/>
+      <c r="AE3" s="29"/>
+      <c r="AF3" s="29"/>
+      <c r="AG3" s="29"/>
+      <c r="AH3" s="29"/>
+      <c r="AI3" s="29"/>
+      <c r="AJ3" s="29"/>
+      <c r="AK3" s="29"/>
+      <c r="AL3" s="29"/>
+      <c r="AM3" s="29"/>
+      <c r="AN3" s="29"/>
+      <c r="AO3" s="29"/>
+      <c r="AP3" s="29"/>
+      <c r="AQ3" s="29"/>
+      <c r="AR3" s="29"/>
+      <c r="AS3" s="29"/>
+      <c r="AT3" s="29"/>
     </row>
     <row r="4" ht="14.6" customHeight="1">
-      <c r="A4" s="8">
+      <c r="A4" s="27">
         <v>2</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" t="s" s="7">
-        <v>215</v>
-      </c>
-      <c r="D4" t="s" s="7">
-        <v>216</v>
-      </c>
-      <c r="E4" t="s" s="12">
-        <v>223</v>
-      </c>
-      <c r="F4" t="s" s="7">
+      <c r="B4" s="29"/>
+      <c r="C4" t="s" s="26">
         <v>218</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" t="s" s="12">
+      <c r="D4" t="s" s="26">
+        <v>219</v>
+      </c>
+      <c r="E4" t="s" s="31">
+        <v>226</v>
+      </c>
+      <c r="F4" t="s" s="26">
+        <v>221</v>
+      </c>
+      <c r="G4" s="29"/>
+      <c r="H4" t="s" s="31">
+        <v>227</v>
+      </c>
+      <c r="I4" t="s" s="26">
         <v>224</v>
       </c>
-      <c r="I4" t="s" s="7">
-        <v>221</v>
-      </c>
-      <c r="J4" s="14">
+      <c r="J4" s="33">
         <v>25153</v>
       </c>
-      <c r="K4" t="b" s="8">
-        <v>0</v>
-      </c>
-      <c r="L4" s="10"/>
-      <c r="M4" t="s" s="7">
-        <v>222</v>
-      </c>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="10"/>
-      <c r="AC4" s="10"/>
-      <c r="AD4" s="10"/>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="10"/>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="10"/>
-      <c r="AL4" s="10"/>
-      <c r="AM4" s="10"/>
-      <c r="AN4" s="10"/>
-      <c r="AO4" s="10"/>
-      <c r="AP4" s="10"/>
-      <c r="AQ4" s="10"/>
-      <c r="AR4" s="10"/>
-      <c r="AS4" s="10"/>
-      <c r="AT4" s="10"/>
+      <c r="K4" t="b" s="27">
+        <v>0</v>
+      </c>
+      <c r="L4" s="29"/>
+      <c r="M4" t="s" s="26">
+        <v>225</v>
+      </c>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="29"/>
+      <c r="W4" s="29"/>
+      <c r="X4" s="29"/>
+      <c r="Y4" s="29"/>
+      <c r="Z4" s="29"/>
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="29"/>
+      <c r="AC4" s="29"/>
+      <c r="AD4" s="29"/>
+      <c r="AE4" s="29"/>
+      <c r="AF4" s="29"/>
+      <c r="AG4" s="29"/>
+      <c r="AH4" s="29"/>
+      <c r="AI4" s="29"/>
+      <c r="AJ4" s="29"/>
+      <c r="AK4" s="29"/>
+      <c r="AL4" s="29"/>
+      <c r="AM4" s="29"/>
+      <c r="AN4" s="29"/>
+      <c r="AO4" s="29"/>
+      <c r="AP4" s="29"/>
+      <c r="AQ4" s="29"/>
+      <c r="AR4" s="29"/>
+      <c r="AS4" s="29"/>
+      <c r="AT4" s="29"/>
     </row>
     <row r="5" ht="14.6" customHeight="1">
-      <c r="A5" s="8">
+      <c r="A5" s="27">
         <v>2</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" t="s" s="7">
+      <c r="B5" s="29"/>
+      <c r="C5" t="s" s="26">
+        <v>228</v>
+      </c>
+      <c r="D5" t="s" s="26">
+        <v>219</v>
+      </c>
+      <c r="E5" t="s" s="26">
+        <v>229</v>
+      </c>
+      <c r="F5" t="s" s="26">
+        <v>230</v>
+      </c>
+      <c r="G5" s="29"/>
+      <c r="H5" t="s" s="26">
+        <v>227</v>
+      </c>
+      <c r="I5" t="s" s="26">
+        <v>231</v>
+      </c>
+      <c r="J5" s="33">
+        <v>27001</v>
+      </c>
+      <c r="K5" t="b" s="27">
+        <v>0</v>
+      </c>
+      <c r="L5" s="29"/>
+      <c r="M5" t="s" s="26">
         <v>225</v>
       </c>
-      <c r="D5" t="s" s="7">
-        <v>216</v>
-      </c>
-      <c r="E5" t="s" s="7">
-        <v>226</v>
-      </c>
-      <c r="F5" t="s" s="7">
-        <v>227</v>
-      </c>
-      <c r="G5" s="10"/>
-      <c r="H5" t="s" s="7">
-        <v>224</v>
-      </c>
-      <c r="I5" t="s" s="7">
-        <v>228</v>
-      </c>
-      <c r="J5" s="14">
-        <v>27001</v>
-      </c>
-      <c r="K5" t="b" s="8">
-        <v>0</v>
-      </c>
-      <c r="L5" s="10"/>
-      <c r="M5" t="s" s="7">
-        <v>222</v>
-      </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10"/>
-      <c r="Z5" s="10"/>
-      <c r="AA5" s="10"/>
-      <c r="AB5" s="10"/>
-      <c r="AC5" s="10"/>
-      <c r="AD5" s="10"/>
-      <c r="AE5" s="10"/>
-      <c r="AF5" s="10"/>
-      <c r="AG5" s="10"/>
-      <c r="AH5" s="10"/>
-      <c r="AI5" s="10"/>
-      <c r="AJ5" s="10"/>
-      <c r="AK5" s="10"/>
-      <c r="AL5" s="10"/>
-      <c r="AM5" s="10"/>
-      <c r="AN5" s="10"/>
-      <c r="AO5" s="10"/>
-      <c r="AP5" s="10"/>
-      <c r="AQ5" s="10"/>
-      <c r="AR5" s="10"/>
-      <c r="AS5" s="10"/>
-      <c r="AT5" s="10"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="29"/>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="29"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="29"/>
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="29"/>
+      <c r="AD5" s="29"/>
+      <c r="AE5" s="29"/>
+      <c r="AF5" s="29"/>
+      <c r="AG5" s="29"/>
+      <c r="AH5" s="29"/>
+      <c r="AI5" s="29"/>
+      <c r="AJ5" s="29"/>
+      <c r="AK5" s="29"/>
+      <c r="AL5" s="29"/>
+      <c r="AM5" s="29"/>
+      <c r="AN5" s="29"/>
+      <c r="AO5" s="29"/>
+      <c r="AP5" s="29"/>
+      <c r="AQ5" s="29"/>
+      <c r="AR5" s="29"/>
+      <c r="AS5" s="29"/>
+      <c r="AT5" s="29"/>
     </row>
     <row r="6" ht="14.6" customHeight="1">
-      <c r="A6" s="8">
+      <c r="A6" s="27">
         <v>3</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" t="s" s="7">
-        <v>215</v>
-      </c>
-      <c r="D6" t="s" s="7">
-        <v>216</v>
-      </c>
-      <c r="E6" t="s" s="7">
-        <v>229</v>
-      </c>
-      <c r="F6" t="s" s="7">
+      <c r="B6" s="29"/>
+      <c r="C6" t="s" s="26">
+        <v>218</v>
+      </c>
+      <c r="D6" t="s" s="26">
+        <v>219</v>
+      </c>
+      <c r="E6" t="s" s="26">
+        <v>232</v>
+      </c>
+      <c r="F6" t="s" s="26">
+        <v>233</v>
+      </c>
+      <c r="G6" s="29"/>
+      <c r="H6" t="s" s="26">
         <v>230</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" t="s" s="7">
-        <v>227</v>
-      </c>
-      <c r="I6" t="s" s="7">
-        <v>221</v>
-      </c>
-      <c r="J6" s="14">
+      <c r="I6" t="s" s="26">
+        <v>224</v>
+      </c>
+      <c r="J6" s="33">
         <v>20857</v>
       </c>
-      <c r="K6" t="b" s="8">
-        <v>0</v>
-      </c>
-      <c r="L6" s="10"/>
-      <c r="M6" t="s" s="7">
-        <v>222</v>
-      </c>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="10"/>
-      <c r="AB6" s="10"/>
-      <c r="AC6" s="10"/>
-      <c r="AD6" s="10"/>
-      <c r="AE6" s="10"/>
-      <c r="AF6" s="10"/>
-      <c r="AG6" s="10"/>
-      <c r="AH6" s="10"/>
-      <c r="AI6" s="10"/>
-      <c r="AJ6" s="10"/>
-      <c r="AK6" s="10"/>
-      <c r="AL6" s="10"/>
-      <c r="AM6" s="10"/>
-      <c r="AN6" s="10"/>
-      <c r="AO6" s="10"/>
-      <c r="AP6" s="10"/>
-      <c r="AQ6" s="10"/>
-      <c r="AR6" s="10"/>
-      <c r="AS6" s="10"/>
-      <c r="AT6" s="10"/>
+      <c r="K6" t="b" s="27">
+        <v>0</v>
+      </c>
+      <c r="L6" s="29"/>
+      <c r="M6" t="s" s="26">
+        <v>225</v>
+      </c>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="29"/>
+      <c r="X6" s="29"/>
+      <c r="Y6" s="29"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="29"/>
+      <c r="AB6" s="29"/>
+      <c r="AC6" s="29"/>
+      <c r="AD6" s="29"/>
+      <c r="AE6" s="29"/>
+      <c r="AF6" s="29"/>
+      <c r="AG6" s="29"/>
+      <c r="AH6" s="29"/>
+      <c r="AI6" s="29"/>
+      <c r="AJ6" s="29"/>
+      <c r="AK6" s="29"/>
+      <c r="AL6" s="29"/>
+      <c r="AM6" s="29"/>
+      <c r="AN6" s="29"/>
+      <c r="AO6" s="29"/>
+      <c r="AP6" s="29"/>
+      <c r="AQ6" s="29"/>
+      <c r="AR6" s="29"/>
+      <c r="AS6" s="29"/>
+      <c r="AT6" s="29"/>
     </row>
     <row r="7" ht="14.6" customHeight="1">
-      <c r="A7" s="8">
+      <c r="A7" s="27">
         <v>3</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" t="s" s="7">
+      <c r="B7" s="29"/>
+      <c r="C7" t="s" s="26">
+        <v>228</v>
+      </c>
+      <c r="D7" t="s" s="26">
+        <v>219</v>
+      </c>
+      <c r="E7" t="s" s="26">
+        <v>234</v>
+      </c>
+      <c r="F7" t="s" s="26">
+        <v>235</v>
+      </c>
+      <c r="G7" s="29"/>
+      <c r="H7" t="s" s="26">
+        <v>230</v>
+      </c>
+      <c r="I7" t="s" s="26">
+        <v>231</v>
+      </c>
+      <c r="J7" s="33">
+        <v>23045</v>
+      </c>
+      <c r="K7" t="b" s="27">
+        <v>0</v>
+      </c>
+      <c r="L7" s="29"/>
+      <c r="M7" t="s" s="26">
         <v>225</v>
       </c>
-      <c r="D7" t="s" s="7">
-        <v>216</v>
-      </c>
-      <c r="E7" t="s" s="7">
-        <v>231</v>
-      </c>
-      <c r="F7" t="s" s="7">
-        <v>232</v>
-      </c>
-      <c r="G7" s="10"/>
-      <c r="H7" t="s" s="7">
-        <v>227</v>
-      </c>
-      <c r="I7" t="s" s="7">
-        <v>228</v>
-      </c>
-      <c r="J7" s="14">
-        <v>23045</v>
-      </c>
-      <c r="K7" t="b" s="8">
-        <v>0</v>
-      </c>
-      <c r="L7" s="10"/>
-      <c r="M7" t="s" s="7">
-        <v>222</v>
-      </c>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="10"/>
-      <c r="Z7" s="10"/>
-      <c r="AA7" s="10"/>
-      <c r="AB7" s="10"/>
-      <c r="AC7" s="10"/>
-      <c r="AD7" s="10"/>
-      <c r="AE7" s="10"/>
-      <c r="AF7" s="10"/>
-      <c r="AG7" s="10"/>
-      <c r="AH7" s="10"/>
-      <c r="AI7" s="10"/>
-      <c r="AJ7" s="10"/>
-      <c r="AK7" s="10"/>
-      <c r="AL7" s="10"/>
-      <c r="AM7" s="10"/>
-      <c r="AN7" s="10"/>
-      <c r="AO7" s="10"/>
-      <c r="AP7" s="10"/>
-      <c r="AQ7" s="10"/>
-      <c r="AR7" s="10"/>
-      <c r="AS7" s="10"/>
-      <c r="AT7" s="10"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="29"/>
+      <c r="AB7" s="29"/>
+      <c r="AC7" s="29"/>
+      <c r="AD7" s="29"/>
+      <c r="AE7" s="29"/>
+      <c r="AF7" s="29"/>
+      <c r="AG7" s="29"/>
+      <c r="AH7" s="29"/>
+      <c r="AI7" s="29"/>
+      <c r="AJ7" s="29"/>
+      <c r="AK7" s="29"/>
+      <c r="AL7" s="29"/>
+      <c r="AM7" s="29"/>
+      <c r="AN7" s="29"/>
+      <c r="AO7" s="29"/>
+      <c r="AP7" s="29"/>
+      <c r="AQ7" s="29"/>
+      <c r="AR7" s="29"/>
+      <c r="AS7" s="29"/>
+      <c r="AT7" s="29"/>
     </row>
     <row r="8" ht="14.6" customHeight="1">
-      <c r="A8" s="8">
+      <c r="A8" s="27">
         <v>3</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" t="s" s="7">
+      <c r="B8" s="29"/>
+      <c r="C8" t="s" s="26">
+        <v>228</v>
+      </c>
+      <c r="D8" t="s" s="26">
+        <v>219</v>
+      </c>
+      <c r="E8" t="s" s="26">
+        <v>236</v>
+      </c>
+      <c r="F8" t="s" s="26">
+        <v>237</v>
+      </c>
+      <c r="G8" s="29"/>
+      <c r="H8" t="s" s="26">
+        <v>230</v>
+      </c>
+      <c r="I8" t="s" s="26">
+        <v>231</v>
+      </c>
+      <c r="J8" s="33">
+        <v>23073</v>
+      </c>
+      <c r="K8" t="b" s="27">
+        <v>0</v>
+      </c>
+      <c r="L8" s="29"/>
+      <c r="M8" t="s" s="26">
         <v>225</v>
       </c>
-      <c r="D8" t="s" s="7">
-        <v>216</v>
-      </c>
-      <c r="E8" t="s" s="7">
-        <v>233</v>
-      </c>
-      <c r="F8" t="s" s="7">
-        <v>234</v>
-      </c>
-      <c r="G8" s="10"/>
-      <c r="H8" t="s" s="7">
-        <v>227</v>
-      </c>
-      <c r="I8" t="s" s="7">
-        <v>228</v>
-      </c>
-      <c r="J8" s="14">
-        <v>23073</v>
-      </c>
-      <c r="K8" t="b" s="8">
-        <v>0</v>
-      </c>
-      <c r="L8" s="10"/>
-      <c r="M8" t="s" s="7">
-        <v>222</v>
-      </c>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="10"/>
-      <c r="AA8" s="10"/>
-      <c r="AB8" s="10"/>
-      <c r="AC8" s="10"/>
-      <c r="AD8" s="10"/>
-      <c r="AE8" s="10"/>
-      <c r="AF8" s="10"/>
-      <c r="AG8" s="10"/>
-      <c r="AH8" s="10"/>
-      <c r="AI8" s="10"/>
-      <c r="AJ8" s="10"/>
-      <c r="AK8" s="10"/>
-      <c r="AL8" s="10"/>
-      <c r="AM8" s="10"/>
-      <c r="AN8" s="10"/>
-      <c r="AO8" s="10"/>
-      <c r="AP8" s="10"/>
-      <c r="AQ8" s="10"/>
-      <c r="AR8" s="10"/>
-      <c r="AS8" s="10"/>
-      <c r="AT8" s="10"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="29"/>
+      <c r="V8" s="29"/>
+      <c r="W8" s="29"/>
+      <c r="X8" s="29"/>
+      <c r="Y8" s="29"/>
+      <c r="Z8" s="29"/>
+      <c r="AA8" s="29"/>
+      <c r="AB8" s="29"/>
+      <c r="AC8" s="29"/>
+      <c r="AD8" s="29"/>
+      <c r="AE8" s="29"/>
+      <c r="AF8" s="29"/>
+      <c r="AG8" s="29"/>
+      <c r="AH8" s="29"/>
+      <c r="AI8" s="29"/>
+      <c r="AJ8" s="29"/>
+      <c r="AK8" s="29"/>
+      <c r="AL8" s="29"/>
+      <c r="AM8" s="29"/>
+      <c r="AN8" s="29"/>
+      <c r="AO8" s="29"/>
+      <c r="AP8" s="29"/>
+      <c r="AQ8" s="29"/>
+      <c r="AR8" s="29"/>
+      <c r="AS8" s="29"/>
+      <c r="AT8" s="29"/>
     </row>
     <row r="9" ht="14.6" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="10"/>
-      <c r="AA9" s="10"/>
-      <c r="AB9" s="10"/>
-      <c r="AC9" s="10"/>
-      <c r="AD9" s="10"/>
-      <c r="AE9" s="10"/>
-      <c r="AF9" s="10"/>
-      <c r="AG9" s="10"/>
-      <c r="AH9" s="10"/>
-      <c r="AI9" s="10"/>
-      <c r="AJ9" s="10"/>
-      <c r="AK9" s="10"/>
-      <c r="AL9" s="10"/>
-      <c r="AM9" s="10"/>
-      <c r="AN9" s="10"/>
-      <c r="AO9" s="10"/>
-      <c r="AP9" s="10"/>
-      <c r="AQ9" s="10"/>
-      <c r="AR9" s="10"/>
-      <c r="AS9" s="10"/>
-      <c r="AT9" s="10"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="29"/>
+      <c r="X9" s="29"/>
+      <c r="Y9" s="29"/>
+      <c r="Z9" s="29"/>
+      <c r="AA9" s="29"/>
+      <c r="AB9" s="29"/>
+      <c r="AC9" s="29"/>
+      <c r="AD9" s="29"/>
+      <c r="AE9" s="29"/>
+      <c r="AF9" s="29"/>
+      <c r="AG9" s="29"/>
+      <c r="AH9" s="29"/>
+      <c r="AI9" s="29"/>
+      <c r="AJ9" s="29"/>
+      <c r="AK9" s="29"/>
+      <c r="AL9" s="29"/>
+      <c r="AM9" s="29"/>
+      <c r="AN9" s="29"/>
+      <c r="AO9" s="29"/>
+      <c r="AP9" s="29"/>
+      <c r="AQ9" s="29"/>
+      <c r="AR9" s="29"/>
+      <c r="AS9" s="29"/>
+      <c r="AT9" s="29"/>
     </row>
     <row r="10" ht="14.6" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="10"/>
-      <c r="AA10" s="10"/>
-      <c r="AB10" s="10"/>
-      <c r="AC10" s="10"/>
-      <c r="AD10" s="10"/>
-      <c r="AE10" s="10"/>
-      <c r="AF10" s="10"/>
-      <c r="AG10" s="10"/>
-      <c r="AH10" s="10"/>
-      <c r="AI10" s="10"/>
-      <c r="AJ10" s="10"/>
-      <c r="AK10" s="10"/>
-      <c r="AL10" s="10"/>
-      <c r="AM10" s="10"/>
-      <c r="AN10" s="10"/>
-      <c r="AO10" s="10"/>
-      <c r="AP10" s="10"/>
-      <c r="AQ10" s="10"/>
-      <c r="AR10" s="10"/>
-      <c r="AS10" s="10"/>
-      <c r="AT10" s="10"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="29"/>
+      <c r="W10" s="29"/>
+      <c r="X10" s="29"/>
+      <c r="Y10" s="29"/>
+      <c r="Z10" s="29"/>
+      <c r="AA10" s="29"/>
+      <c r="AB10" s="29"/>
+      <c r="AC10" s="29"/>
+      <c r="AD10" s="29"/>
+      <c r="AE10" s="29"/>
+      <c r="AF10" s="29"/>
+      <c r="AG10" s="29"/>
+      <c r="AH10" s="29"/>
+      <c r="AI10" s="29"/>
+      <c r="AJ10" s="29"/>
+      <c r="AK10" s="29"/>
+      <c r="AL10" s="29"/>
+      <c r="AM10" s="29"/>
+      <c r="AN10" s="29"/>
+      <c r="AO10" s="29"/>
+      <c r="AP10" s="29"/>
+      <c r="AQ10" s="29"/>
+      <c r="AR10" s="29"/>
+      <c r="AS10" s="29"/>
+      <c r="AT10" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>

</xml_diff>

<commit_message>
part 2: xlsx rdi logic and unit tests fix
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/registration_datahub/tests/test_file/new_reg_data_import.xlsx
+++ b/backend/hct_mis_api/apps/registration_datahub/tests/test_file/new_reg_data_import.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="235">
   <si>
     <t>household_id</t>
   </si>
@@ -389,7 +389,10 @@
     <t>relationship_i_c</t>
   </si>
   <si>
-    <t>role_i_c</t>
+    <t>primary_collector_id</t>
+  </si>
+  <si>
+    <t>alternate_collector_id</t>
   </si>
   <si>
     <t>full_name_i_c</t>
@@ -653,7 +656,7 @@
     <t>HEAD</t>
   </si>
   <si>
-    <t>PRIMARY</t>
+    <t>1</t>
   </si>
   <si>
     <t>Some Full Name</t>
@@ -674,6 +677,9 @@
     <t>MARRIED</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>Some Ipsum</t>
   </si>
   <si>
@@ -690,6 +696,9 @@
   </si>
   <si>
     <t>FEMALE</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
   <si>
     <t>Name1 Lorem</t>
@@ -3117,7 +3126,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AU10"/>
+  <dimension ref="A1:AV10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -3126,50 +3135,51 @@
     <col min="1" max="1" width="10.8516" style="9" customWidth="1"/>
     <col min="2" max="3" width="12.6719" style="9" customWidth="1"/>
     <col min="4" max="4" width="33.8516" style="9" customWidth="1"/>
-    <col min="5" max="5" width="7.85156" style="9" customWidth="1"/>
-    <col min="6" max="6" width="15.8516" style="9" customWidth="1"/>
-    <col min="7" max="7" width="12.8516" style="9" customWidth="1"/>
-    <col min="8" max="8" width="14" style="9" customWidth="1"/>
-    <col min="9" max="9" width="13.3516" style="9" customWidth="1"/>
-    <col min="10" max="10" width="11" style="9" customWidth="1"/>
-    <col min="11" max="11" width="15.8516" style="9" customWidth="1"/>
-    <col min="12" max="12" width="19.8516" style="9" customWidth="1"/>
-    <col min="13" max="13" width="8.35156" style="9" customWidth="1"/>
-    <col min="14" max="14" width="18.8516" style="9" customWidth="1"/>
-    <col min="15" max="15" width="11.8516" style="9" customWidth="1"/>
-    <col min="16" max="16" width="20.3516" style="9" customWidth="1"/>
-    <col min="17" max="17" width="18.3516" style="9" customWidth="1"/>
-    <col min="18" max="18" width="20.8516" style="9" customWidth="1"/>
-    <col min="19" max="19" width="18.1719" style="9" customWidth="1"/>
-    <col min="20" max="20" width="20" style="9" customWidth="1"/>
-    <col min="21" max="21" width="17.1719" style="9" customWidth="1"/>
-    <col min="22" max="22" width="19.5" style="9" customWidth="1"/>
-    <col min="23" max="23" width="14.5" style="9" customWidth="1"/>
-    <col min="24" max="24" width="15.6719" style="9" customWidth="1"/>
-    <col min="25" max="25" width="20" style="9" customWidth="1"/>
-    <col min="26" max="26" width="22.3516" style="9" customWidth="1"/>
-    <col min="27" max="27" width="17.3516" style="9" customWidth="1"/>
-    <col min="28" max="28" width="15.8516" style="9" customWidth="1"/>
-    <col min="29" max="29" width="14.3516" style="9" customWidth="1"/>
-    <col min="30" max="30" width="13" style="9" customWidth="1"/>
-    <col min="31" max="31" width="8.17188" style="9" customWidth="1"/>
-    <col min="32" max="32" width="37.5" style="9" customWidth="1"/>
-    <col min="33" max="33" width="14.1719" style="9" customWidth="1"/>
-    <col min="34" max="34" width="31.3516" style="9" customWidth="1"/>
-    <col min="35" max="35" width="39.1719" style="9" customWidth="1"/>
-    <col min="36" max="36" width="40" style="9" customWidth="1"/>
-    <col min="37" max="37" width="52.6719" style="9" customWidth="1"/>
-    <col min="38" max="38" width="56.8516" style="9" customWidth="1"/>
-    <col min="39" max="39" width="54.1719" style="9" customWidth="1"/>
-    <col min="40" max="40" width="45.6719" style="9" customWidth="1"/>
-    <col min="41" max="41" width="35.3516" style="9" customWidth="1"/>
-    <col min="42" max="42" width="32.8516" style="9" customWidth="1"/>
-    <col min="43" max="43" width="46.8516" style="9" customWidth="1"/>
-    <col min="44" max="44" width="45.1719" style="9" customWidth="1"/>
-    <col min="45" max="45" width="16.3516" style="9" customWidth="1"/>
-    <col min="46" max="46" width="34.3516" style="9" customWidth="1"/>
-    <col min="47" max="47" width="60.3516" style="9" customWidth="1"/>
-    <col min="48" max="16384" width="12.6719" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="9" customWidth="1"/>
+    <col min="6" max="6" width="17.3516" style="9" customWidth="1"/>
+    <col min="7" max="7" width="15.8516" style="9" customWidth="1"/>
+    <col min="8" max="8" width="12.8516" style="9" customWidth="1"/>
+    <col min="9" max="9" width="14" style="9" customWidth="1"/>
+    <col min="10" max="10" width="13.3516" style="9" customWidth="1"/>
+    <col min="11" max="11" width="11" style="9" customWidth="1"/>
+    <col min="12" max="12" width="15.8516" style="9" customWidth="1"/>
+    <col min="13" max="13" width="19.8516" style="9" customWidth="1"/>
+    <col min="14" max="14" width="8.35156" style="9" customWidth="1"/>
+    <col min="15" max="15" width="18.8516" style="9" customWidth="1"/>
+    <col min="16" max="16" width="11.8516" style="9" customWidth="1"/>
+    <col min="17" max="17" width="20.3516" style="9" customWidth="1"/>
+    <col min="18" max="18" width="18.3516" style="9" customWidth="1"/>
+    <col min="19" max="19" width="20.8516" style="9" customWidth="1"/>
+    <col min="20" max="20" width="18.1719" style="9" customWidth="1"/>
+    <col min="21" max="21" width="20" style="9" customWidth="1"/>
+    <col min="22" max="22" width="17.1719" style="9" customWidth="1"/>
+    <col min="23" max="23" width="19.5" style="9" customWidth="1"/>
+    <col min="24" max="24" width="14.5" style="9" customWidth="1"/>
+    <col min="25" max="25" width="15.6719" style="9" customWidth="1"/>
+    <col min="26" max="26" width="20" style="9" customWidth="1"/>
+    <col min="27" max="27" width="22.3516" style="9" customWidth="1"/>
+    <col min="28" max="28" width="17.3516" style="9" customWidth="1"/>
+    <col min="29" max="29" width="15.8516" style="9" customWidth="1"/>
+    <col min="30" max="30" width="14.3516" style="9" customWidth="1"/>
+    <col min="31" max="31" width="13" style="9" customWidth="1"/>
+    <col min="32" max="32" width="8.17188" style="9" customWidth="1"/>
+    <col min="33" max="33" width="37.5" style="9" customWidth="1"/>
+    <col min="34" max="34" width="14.1719" style="9" customWidth="1"/>
+    <col min="35" max="35" width="31.3516" style="9" customWidth="1"/>
+    <col min="36" max="36" width="39.1719" style="9" customWidth="1"/>
+    <col min="37" max="37" width="40" style="9" customWidth="1"/>
+    <col min="38" max="38" width="52.6719" style="9" customWidth="1"/>
+    <col min="39" max="39" width="56.8516" style="9" customWidth="1"/>
+    <col min="40" max="40" width="54.1719" style="9" customWidth="1"/>
+    <col min="41" max="41" width="45.6719" style="9" customWidth="1"/>
+    <col min="42" max="42" width="35.3516" style="9" customWidth="1"/>
+    <col min="43" max="43" width="32.8516" style="9" customWidth="1"/>
+    <col min="44" max="44" width="46.8516" style="9" customWidth="1"/>
+    <col min="45" max="45" width="45.1719" style="9" customWidth="1"/>
+    <col min="46" max="46" width="16.3516" style="9" customWidth="1"/>
+    <col min="47" max="47" width="34.3516" style="9" customWidth="1"/>
+    <col min="48" max="48" width="60.3516" style="9" customWidth="1"/>
+    <col min="49" max="16384" width="12.6719" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -3314,22 +3324,25 @@
       <c r="AU1" t="s" s="2">
         <v>167</v>
       </c>
+      <c r="AV1" t="s" s="2">
+        <v>168</v>
+      </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
         <v>59</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F2" t="s" s="2">
         <v>172</v>
@@ -3407,16 +3420,16 @@
         <v>196</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="AF2" t="s" s="2">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="AG2" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="AH2" t="s" s="2">
         <v>95</v>
-      </c>
-      <c r="AH2" t="s" s="2">
-        <v>198</v>
       </c>
       <c r="AI2" t="s" s="2">
         <v>199</v>
@@ -3456,6 +3469,9 @@
       </c>
       <c r="AU2" t="s" s="2">
         <v>211</v>
+      </c>
+      <c r="AV2" t="s" s="2">
+        <v>212</v>
       </c>
     </row>
     <row r="3" ht="14.6" customHeight="1">
@@ -3467,15 +3483,13 @@
         <v>43864</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>213</v>
-      </c>
-      <c r="F3" t="s" s="8">
         <v>214</v>
       </c>
-      <c r="G3" t="s" s="2">
+      <c r="F3" s="2"/>
+      <c r="G3" t="s" s="8">
         <v>215</v>
       </c>
       <c r="H3" t="s" s="2">
@@ -3487,17 +3501,19 @@
       <c r="J3" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="L3" s="6">
         <v>23045</v>
       </c>
-      <c r="L3" t="b" s="3">
-        <v>0</v>
-      </c>
-      <c r="M3" s="5"/>
-      <c r="N3" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="O3" s="5"/>
+      <c r="M3" t="b" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5"/>
+      <c r="O3" t="s" s="2">
+        <v>220</v>
+      </c>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
@@ -3530,6 +3546,7 @@
       <c r="AS3" s="5"/>
       <c r="AT3" s="5"/>
       <c r="AU3" s="5"/>
+      <c r="AV3" s="5"/>
     </row>
     <row r="4" ht="14.6" customHeight="1">
       <c r="A4" s="3">
@@ -3540,35 +3557,35 @@
         <v>43865</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E4" t="s" s="2">
-        <v>213</v>
-      </c>
-      <c r="F4" t="s" s="8">
+        <v>221</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" t="s" s="8">
+        <v>222</v>
+      </c>
+      <c r="H4" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" t="s" s="8">
+        <v>223</v>
+      </c>
+      <c r="K4" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="L4" s="6">
+        <v>25153</v>
+      </c>
+      <c r="M4" t="b" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" t="s" s="2">
         <v>220</v>
       </c>
-      <c r="G4" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" t="s" s="8">
-        <v>221</v>
-      </c>
-      <c r="J4" t="s" s="2">
-        <v>218</v>
-      </c>
-      <c r="K4" s="6">
-        <v>25153</v>
-      </c>
-      <c r="L4" t="b" s="3">
-        <v>0</v>
-      </c>
-      <c r="M4" s="5"/>
-      <c r="N4" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="O4" s="5"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
@@ -3601,6 +3618,7 @@
       <c r="AS4" s="5"/>
       <c r="AT4" s="5"/>
       <c r="AU4" s="5"/>
+      <c r="AV4" s="5"/>
     </row>
     <row r="5" ht="14.6" customHeight="1">
       <c r="A5" s="3">
@@ -3611,35 +3629,35 @@
         <v>43866</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="E5" t="s" s="2">
-        <v>213</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="E5" s="2"/>
       <c r="F5" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="G5" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="H5" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" t="s" s="2">
         <v>223</v>
       </c>
-      <c r="G5" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="J5" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="K5" s="6">
+      <c r="K5" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="L5" s="6">
         <v>27001</v>
       </c>
-      <c r="L5" t="b" s="3">
-        <v>0</v>
-      </c>
-      <c r="M5" s="5"/>
-      <c r="N5" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="O5" s="5"/>
+      <c r="M5" t="b" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5"/>
+      <c r="O5" t="s" s="2">
+        <v>220</v>
+      </c>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
@@ -3672,6 +3690,7 @@
       <c r="AS5" s="5"/>
       <c r="AT5" s="5"/>
       <c r="AU5" s="5"/>
+      <c r="AV5" s="5"/>
     </row>
     <row r="6" ht="14.6" customHeight="1">
       <c r="A6" s="3">
@@ -3682,35 +3701,35 @@
         <v>43867</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E6" t="s" s="2">
-        <v>213</v>
-      </c>
-      <c r="F6" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="H6" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="G6" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="H6" s="5"/>
-      <c r="I6" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="J6" t="s" s="2">
-        <v>218</v>
-      </c>
-      <c r="K6" s="6">
+      <c r="K6" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="L6" s="6">
         <v>20857</v>
       </c>
-      <c r="L6" t="b" s="3">
-        <v>0</v>
-      </c>
-      <c r="M6" s="5"/>
-      <c r="N6" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="O6" s="5"/>
+      <c r="M6" t="b" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5"/>
+      <c r="O6" t="s" s="2">
+        <v>220</v>
+      </c>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
@@ -3743,6 +3762,7 @@
       <c r="AS6" s="5"/>
       <c r="AT6" s="5"/>
       <c r="AU6" s="5"/>
+      <c r="AV6" s="5"/>
     </row>
     <row r="7" ht="14.6" customHeight="1">
       <c r="A7" s="3">
@@ -3753,35 +3773,35 @@
         <v>43868</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="E7" t="s" s="2">
-        <v>213</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="E7" s="2"/>
       <c r="F7" t="s" s="2">
         <v>228</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="H7" s="5"/>
-      <c r="I7" t="s" s="2">
-        <v>224</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="H7" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="I7" s="5"/>
       <c r="J7" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="K7" s="6">
+        <v>226</v>
+      </c>
+      <c r="K7" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="L7" s="6">
         <v>23045</v>
       </c>
-      <c r="L7" t="b" s="3">
-        <v>0</v>
-      </c>
-      <c r="M7" s="5"/>
-      <c r="N7" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="O7" s="5"/>
+      <c r="M7" t="b" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5"/>
+      <c r="O7" t="s" s="2">
+        <v>220</v>
+      </c>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
@@ -3814,6 +3834,7 @@
       <c r="AS7" s="5"/>
       <c r="AT7" s="5"/>
       <c r="AU7" s="5"/>
+      <c r="AV7" s="5"/>
     </row>
     <row r="8" ht="14.6" customHeight="1">
       <c r="A8" s="3">
@@ -3824,35 +3845,33 @@
         <v>43869</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="E8" t="s" s="2">
-        <v>213</v>
-      </c>
-      <c r="F8" t="s" s="2">
-        <v>230</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
       <c r="G8" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="H8" s="5"/>
-      <c r="I8" t="s" s="2">
-        <v>224</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="H8" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="I8" s="5"/>
       <c r="J8" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="K8" s="6">
+        <v>226</v>
+      </c>
+      <c r="K8" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="L8" s="6">
         <v>23073</v>
       </c>
-      <c r="L8" t="b" s="3">
-        <v>0</v>
-      </c>
-      <c r="M8" s="5"/>
-      <c r="N8" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="O8" s="5"/>
+      <c r="M8" t="b" s="3">
+        <v>0</v>
+      </c>
+      <c r="N8" s="5"/>
+      <c r="O8" t="s" s="2">
+        <v>220</v>
+      </c>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
@@ -3885,6 +3904,7 @@
       <c r="AS8" s="5"/>
       <c r="AT8" s="5"/>
       <c r="AU8" s="5"/>
+      <c r="AV8" s="5"/>
     </row>
     <row r="9" ht="14.6" customHeight="1">
       <c r="A9" s="5"/>
@@ -3934,6 +3954,7 @@
       <c r="AS9" s="5"/>
       <c r="AT9" s="5"/>
       <c r="AU9" s="5"/>
+      <c r="AV9" s="5"/>
     </row>
     <row r="10" ht="14.6" customHeight="1">
       <c r="A10" s="5"/>
@@ -3983,6 +4004,7 @@
       <c r="AS10" s="5"/>
       <c r="AT10" s="5"/>
       <c r="AU10" s="5"/>
+      <c r="AV10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>

</xml_diff>